<commit_message>
corrected stomach zone IDs
</commit_message>
<xml_diff>
--- a/flatmap_annotation.xlsx
+++ b/flatmap_annotation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nebr002\work\sparc\flatmaps\rat\sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nebr002\work\sparc\flatmaps\rat\powerpoint\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9278" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9278"/>
   </bookViews>
   <sheets>
     <sheet name="Body organs" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="1076">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1800" uniqueCount="1083">
   <si>
     <t>Power point identifier</t>
   </si>
@@ -3218,18 +3218,9 @@
     <t>fundus of stomach</t>
   </si>
   <si>
-    <t xml:space="preserve">ILX:0724443 </t>
-  </si>
-  <si>
     <t xml:space="preserve">UBERON:0001160 </t>
   </si>
   <si>
-    <t>murine forestomach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ILX:0729690 </t>
-  </si>
-  <si>
     <t xml:space="preserve">UBERON:0008827 </t>
   </si>
   <si>
@@ -3252,6 +3243,36 @@
   </si>
   <si>
     <t>pylorus</t>
+  </si>
+  <si>
+    <t>body_8</t>
+  </si>
+  <si>
+    <t>tongue</t>
+  </si>
+  <si>
+    <t>respiratory_13</t>
+  </si>
+  <si>
+    <t>nasopharynx</t>
+  </si>
+  <si>
+    <t>arytenoid cartilage</t>
+  </si>
+  <si>
+    <t>respiratory_14</t>
+  </si>
+  <si>
+    <t>body of stomach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0001161 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ILX:0724929</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ILX:0724443 </t>
   </si>
 </sst>
 </file>
@@ -3558,7 +3579,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3666,6 +3687,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3884,10 +3906,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB1048"/>
+  <dimension ref="A1:AB1050"/>
   <sheetViews>
-    <sheetView topLeftCell="E73" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="I89" sqref="I89:I92"/>
+    <sheetView tabSelected="1" topLeftCell="C63" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="H100" sqref="H100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -6067,14 +6089,18 @@
       <c r="R70" s="40"/>
     </row>
     <row r="71" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A71" s="19"/>
-      <c r="B71" s="39"/>
+      <c r="A71" s="44" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B71" s="35"/>
       <c r="C71" s="21"/>
-      <c r="D71" s="23"/>
-      <c r="E71" s="26"/>
+      <c r="D71" s="42" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E71" s="43"/>
       <c r="G71" s="29"/>
-      <c r="H71" s="23"/>
-      <c r="I71" s="26"/>
+      <c r="H71" s="42"/>
+      <c r="I71" s="43"/>
       <c r="K71" s="29"/>
       <c r="L71" s="31"/>
       <c r="M71" s="29"/>
@@ -6084,93 +6110,65 @@
       <c r="R71" s="40"/>
     </row>
     <row r="72" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A72" s="19" t="s">
-        <v>760</v>
-      </c>
-      <c r="B72" s="43" t="s">
-        <v>762</v>
-      </c>
-      <c r="C72" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D72" s="23" t="s">
-        <v>761</v>
-      </c>
-      <c r="E72" s="26" t="s">
-        <v>762</v>
-      </c>
+      <c r="A72" s="35" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B72" s="35"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="67" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E72" s="43"/>
       <c r="G72" s="29"/>
-      <c r="H72" s="42" t="s">
-        <v>761</v>
-      </c>
-      <c r="I72" s="26" t="s">
-        <v>763</v>
-      </c>
+      <c r="H72" s="42"/>
+      <c r="I72" s="43"/>
       <c r="K72" s="29"/>
       <c r="L72" s="31"/>
       <c r="M72" s="29"/>
       <c r="N72" s="33"/>
       <c r="P72" s="29"/>
       <c r="Q72" s="32"/>
-      <c r="R72" s="34" t="s">
-        <v>764</v>
-      </c>
+      <c r="R72" s="40"/>
     </row>
     <row r="73" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A73" s="19" t="s">
-        <v>765</v>
-      </c>
-      <c r="B73" s="43" t="s">
-        <v>767</v>
-      </c>
-      <c r="C73" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D73" s="23" t="s">
-        <v>766</v>
-      </c>
-      <c r="E73" s="26" t="s">
-        <v>767</v>
-      </c>
+      <c r="A73" s="19"/>
+      <c r="B73" s="39"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="26"/>
       <c r="G73" s="29"/>
-      <c r="H73" s="23" t="s">
-        <v>766</v>
-      </c>
-      <c r="I73" s="26" t="s">
-        <v>768</v>
-      </c>
+      <c r="H73" s="23"/>
+      <c r="I73" s="26"/>
       <c r="K73" s="29"/>
       <c r="L73" s="31"/>
       <c r="M73" s="29"/>
       <c r="N73" s="33"/>
       <c r="P73" s="29"/>
       <c r="Q73" s="32"/>
-      <c r="R73" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R73" s="40"/>
     </row>
     <row r="74" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A74" s="19" t="s">
-        <v>769</v>
+        <v>760</v>
       </c>
       <c r="B74" s="43" t="s">
-        <v>771</v>
+        <v>762</v>
       </c>
       <c r="C74" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D74" s="42" t="s">
-        <v>770</v>
+      <c r="D74" s="23" t="s">
+        <v>761</v>
       </c>
       <c r="E74" s="26" t="s">
-        <v>771</v>
+        <v>762</v>
       </c>
       <c r="G74" s="29"/>
       <c r="H74" s="42" t="s">
-        <v>770</v>
+        <v>761</v>
       </c>
       <c r="I74" s="26" t="s">
-        <v>772</v>
+        <v>763</v>
       </c>
       <c r="K74" s="29"/>
       <c r="L74" s="31"/>
@@ -6178,32 +6176,32 @@
       <c r="N74" s="33"/>
       <c r="P74" s="29"/>
       <c r="Q74" s="32"/>
-      <c r="R74" s="34" t="b">
-        <v>1</v>
+      <c r="R74" s="34" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="75" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A75" s="19" t="s">
-        <v>773</v>
+        <v>765</v>
       </c>
       <c r="B75" s="43" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
       <c r="C75" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D75" s="42" t="s">
-        <v>774</v>
+      <c r="D75" s="23" t="s">
+        <v>766</v>
       </c>
       <c r="E75" s="26" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
       <c r="G75" s="29"/>
-      <c r="H75" s="42" t="s">
-        <v>774</v>
+      <c r="H75" s="23" t="s">
+        <v>766</v>
       </c>
       <c r="I75" s="26" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="K75" s="29"/>
       <c r="L75" s="31"/>
@@ -6211,32 +6209,32 @@
       <c r="N75" s="33"/>
       <c r="P75" s="29"/>
       <c r="Q75" s="32"/>
-      <c r="R75" s="34" t="s">
-        <v>95</v>
+      <c r="R75" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A76" s="19" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
       <c r="B76" s="43" t="s">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="C76" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D76" s="23" t="s">
-        <v>778</v>
+      <c r="D76" s="42" t="s">
+        <v>770</v>
       </c>
       <c r="E76" s="26" t="s">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="G76" s="29"/>
-      <c r="H76" s="23" t="s">
-        <v>778</v>
+      <c r="H76" s="42" t="s">
+        <v>770</v>
       </c>
       <c r="I76" s="26" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
       <c r="K76" s="29"/>
       <c r="L76" s="31"/>
@@ -6244,32 +6242,32 @@
       <c r="N76" s="33"/>
       <c r="P76" s="29"/>
       <c r="Q76" s="32"/>
-      <c r="R76" s="34" t="s">
-        <v>33</v>
+      <c r="R76" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A77" s="19" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="B77" s="43" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="C77" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D77" s="23" t="s">
-        <v>782</v>
+      <c r="D77" s="42" t="s">
+        <v>774</v>
       </c>
       <c r="E77" s="26" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="G77" s="29"/>
-      <c r="H77" s="23" t="s">
-        <v>782</v>
+      <c r="H77" s="42" t="s">
+        <v>774</v>
       </c>
       <c r="I77" s="26" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="K77" s="29"/>
       <c r="L77" s="31"/>
@@ -6277,32 +6275,32 @@
       <c r="N77" s="33"/>
       <c r="P77" s="29"/>
       <c r="Q77" s="32"/>
-      <c r="R77" s="34" t="b">
-        <v>1</v>
+      <c r="R77" s="34" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A78" s="19" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="B78" s="43" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
       <c r="C78" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D78" s="23" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
       <c r="E78" s="26" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
       <c r="G78" s="29"/>
       <c r="H78" s="23" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
       <c r="I78" s="26" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="K78" s="29"/>
       <c r="L78" s="31"/>
@@ -6310,32 +6308,32 @@
       <c r="N78" s="33"/>
       <c r="P78" s="29"/>
       <c r="Q78" s="32"/>
-      <c r="R78" s="34" t="b">
-        <v>1</v>
+      <c r="R78" s="34" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="79" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A79" s="19" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
       <c r="B79" s="43" t="s">
-        <v>791</v>
+        <v>783</v>
       </c>
       <c r="C79" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D79" s="23" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
       <c r="E79" s="26" t="s">
-        <v>791</v>
+        <v>783</v>
       </c>
       <c r="G79" s="29"/>
       <c r="H79" s="23" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
       <c r="I79" s="26" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
       <c r="K79" s="29"/>
       <c r="L79" s="31"/>
@@ -6343,32 +6341,32 @@
       <c r="N79" s="33"/>
       <c r="P79" s="29"/>
       <c r="Q79" s="32"/>
-      <c r="R79" s="34" t="s">
-        <v>33</v>
+      <c r="R79" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A80" s="19" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
       <c r="B80" s="43" t="s">
-        <v>795</v>
+        <v>787</v>
       </c>
       <c r="C80" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D80" s="23" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
       <c r="E80" s="26" t="s">
-        <v>795</v>
+        <v>787</v>
       </c>
       <c r="G80" s="29"/>
       <c r="H80" s="23" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
       <c r="I80" s="26" t="s">
-        <v>796</v>
+        <v>788</v>
       </c>
       <c r="K80" s="29"/>
       <c r="L80" s="31"/>
@@ -6382,26 +6380,26 @@
     </row>
     <row r="81" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A81" s="19" t="s">
-        <v>797</v>
+        <v>789</v>
       </c>
       <c r="B81" s="43" t="s">
-        <v>799</v>
+        <v>791</v>
       </c>
       <c r="C81" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D81" s="23" t="s">
-        <v>798</v>
+        <v>790</v>
       </c>
       <c r="E81" s="26" t="s">
-        <v>799</v>
+        <v>791</v>
       </c>
       <c r="G81" s="29"/>
       <c r="H81" s="23" t="s">
-        <v>798</v>
+        <v>790</v>
       </c>
       <c r="I81" s="26" t="s">
-        <v>800</v>
+        <v>792</v>
       </c>
       <c r="K81" s="29"/>
       <c r="L81" s="31"/>
@@ -6409,32 +6407,32 @@
       <c r="N81" s="33"/>
       <c r="P81" s="29"/>
       <c r="Q81" s="32"/>
-      <c r="R81" s="34" t="b">
-        <v>1</v>
+      <c r="R81" s="34" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="82" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A82" s="19" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="B82" s="43" t="s">
-        <v>804</v>
-      </c>
-      <c r="C82" s="50" t="s">
-        <v>802</v>
+        <v>795</v>
+      </c>
+      <c r="C82" s="21" t="s">
+        <v>20</v>
       </c>
       <c r="D82" s="23" t="s">
-        <v>803</v>
+        <v>794</v>
       </c>
       <c r="E82" s="26" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
       <c r="G82" s="29"/>
       <c r="H82" s="23" t="s">
-        <v>803</v>
+        <v>794</v>
       </c>
       <c r="I82" s="26" t="s">
-        <v>805</v>
+        <v>796</v>
       </c>
       <c r="K82" s="29"/>
       <c r="L82" s="31"/>
@@ -6448,26 +6446,26 @@
     </row>
     <row r="83" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A83" s="19" t="s">
-        <v>806</v>
+        <v>797</v>
       </c>
       <c r="B83" s="43" t="s">
-        <v>809</v>
-      </c>
-      <c r="C83" s="50" t="s">
-        <v>807</v>
+        <v>799</v>
+      </c>
+      <c r="C83" s="21" t="s">
+        <v>20</v>
       </c>
       <c r="D83" s="23" t="s">
-        <v>808</v>
+        <v>798</v>
       </c>
       <c r="E83" s="26" t="s">
-        <v>809</v>
+        <v>799</v>
       </c>
       <c r="G83" s="29"/>
       <c r="H83" s="23" t="s">
-        <v>808</v>
+        <v>798</v>
       </c>
       <c r="I83" s="26" t="s">
-        <v>810</v>
+        <v>800</v>
       </c>
       <c r="K83" s="29"/>
       <c r="L83" s="31"/>
@@ -6481,26 +6479,26 @@
     </row>
     <row r="84" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A84" s="19" t="s">
-        <v>811</v>
+        <v>801</v>
       </c>
       <c r="B84" s="43" t="s">
-        <v>813</v>
-      </c>
-      <c r="C84" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D84" s="21" t="s">
-        <v>812</v>
+        <v>804</v>
+      </c>
+      <c r="C84" s="50" t="s">
+        <v>802</v>
+      </c>
+      <c r="D84" s="23" t="s">
+        <v>803</v>
       </c>
       <c r="E84" s="26" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="G84" s="29"/>
       <c r="H84" s="23" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
       <c r="I84" s="26" t="s">
-        <v>814</v>
+        <v>805</v>
       </c>
       <c r="K84" s="29"/>
       <c r="L84" s="31"/>
@@ -6514,26 +6512,26 @@
     </row>
     <row r="85" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A85" s="19" t="s">
-        <v>815</v>
+        <v>806</v>
       </c>
       <c r="B85" s="43" t="s">
-        <v>817</v>
-      </c>
-      <c r="C85" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D85" s="21" t="s">
-        <v>816</v>
+        <v>809</v>
+      </c>
+      <c r="C85" s="50" t="s">
+        <v>807</v>
+      </c>
+      <c r="D85" s="23" t="s">
+        <v>808</v>
       </c>
       <c r="E85" s="26" t="s">
-        <v>817</v>
+        <v>809</v>
       </c>
       <c r="G85" s="29"/>
       <c r="H85" s="23" t="s">
-        <v>816</v>
+        <v>808</v>
       </c>
       <c r="I85" s="26" t="s">
-        <v>818</v>
+        <v>810</v>
       </c>
       <c r="K85" s="29"/>
       <c r="L85" s="31"/>
@@ -6547,26 +6545,26 @@
     </row>
     <row r="86" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A86" s="19" t="s">
-        <v>819</v>
+        <v>811</v>
       </c>
       <c r="B86" s="43" t="s">
-        <v>821</v>
+        <v>813</v>
       </c>
       <c r="C86" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D86" s="21" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
       <c r="E86" s="26" t="s">
-        <v>821</v>
+        <v>813</v>
       </c>
       <c r="G86" s="29"/>
       <c r="H86" s="23" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
       <c r="I86" s="26" t="s">
-        <v>822</v>
+        <v>814</v>
       </c>
       <c r="K86" s="29"/>
       <c r="L86" s="31"/>
@@ -6580,26 +6578,26 @@
     </row>
     <row r="87" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A87" s="19" t="s">
-        <v>823</v>
+        <v>815</v>
       </c>
       <c r="B87" s="43" t="s">
-        <v>825</v>
+        <v>817</v>
       </c>
       <c r="C87" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D87" s="21" t="s">
-        <v>824</v>
+        <v>816</v>
       </c>
       <c r="E87" s="26" t="s">
-        <v>825</v>
+        <v>817</v>
       </c>
       <c r="G87" s="29"/>
       <c r="H87" s="23" t="s">
-        <v>824</v>
+        <v>816</v>
       </c>
       <c r="I87" s="26" t="s">
-        <v>826</v>
+        <v>818</v>
       </c>
       <c r="K87" s="29"/>
       <c r="L87" s="31"/>
@@ -6607,32 +6605,32 @@
       <c r="N87" s="33"/>
       <c r="P87" s="29"/>
       <c r="Q87" s="32"/>
-      <c r="R87" s="34" t="s">
-        <v>827</v>
+      <c r="R87" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A88" s="19" t="s">
-        <v>828</v>
+        <v>819</v>
       </c>
       <c r="B88" s="43" t="s">
-        <v>830</v>
+        <v>821</v>
       </c>
       <c r="C88" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D88" s="21" t="s">
-        <v>829</v>
+        <v>820</v>
       </c>
       <c r="E88" s="26" t="s">
-        <v>830</v>
+        <v>821</v>
       </c>
       <c r="G88" s="29"/>
       <c r="H88" s="23" t="s">
-        <v>829</v>
+        <v>820</v>
       </c>
       <c r="I88" s="26" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
       <c r="K88" s="29"/>
       <c r="L88" s="31"/>
@@ -6640,32 +6638,32 @@
       <c r="N88" s="33"/>
       <c r="P88" s="29"/>
       <c r="Q88" s="32"/>
-      <c r="R88" s="34" t="s">
-        <v>832</v>
+      <c r="R88" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A89" s="65" t="s">
-        <v>1060</v>
+      <c r="A89" s="19" t="s">
+        <v>823</v>
       </c>
       <c r="B89" s="43" t="s">
-        <v>1065</v>
-      </c>
-      <c r="C89" s="59" t="s">
+        <v>825</v>
+      </c>
+      <c r="C89" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D89" s="21" t="s">
-        <v>1063</v>
-      </c>
-      <c r="E89" s="43" t="s">
-        <v>1065</v>
+        <v>824</v>
+      </c>
+      <c r="E89" s="26" t="s">
+        <v>825</v>
       </c>
       <c r="G89" s="29"/>
-      <c r="H89" s="21" t="s">
-        <v>1063</v>
-      </c>
-      <c r="I89" s="43" t="s">
-        <v>1064</v>
+      <c r="H89" s="23" t="s">
+        <v>824</v>
+      </c>
+      <c r="I89" s="26" t="s">
+        <v>826</v>
       </c>
       <c r="K89" s="29"/>
       <c r="L89" s="31"/>
@@ -6673,30 +6671,32 @@
       <c r="N89" s="33"/>
       <c r="P89" s="29"/>
       <c r="Q89" s="32"/>
-      <c r="R89" s="40"/>
+      <c r="R89" s="34" t="s">
+        <v>827</v>
+      </c>
     </row>
     <row r="90" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A90" s="35" t="s">
-        <v>1061</v>
+      <c r="A90" s="19" t="s">
+        <v>828</v>
       </c>
       <c r="B90" s="43" t="s">
-        <v>1068</v>
-      </c>
-      <c r="C90" s="59" t="s">
+        <v>830</v>
+      </c>
+      <c r="C90" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E90" s="43" t="s">
-        <v>1068</v>
+        <v>829</v>
+      </c>
+      <c r="E90" s="26" t="s">
+        <v>830</v>
       </c>
       <c r="G90" s="29"/>
-      <c r="H90" s="21" t="s">
-        <v>1066</v>
-      </c>
-      <c r="I90" s="43" t="s">
-        <v>1067</v>
+      <c r="H90" s="23" t="s">
+        <v>829</v>
+      </c>
+      <c r="I90" s="26" t="s">
+        <v>831</v>
       </c>
       <c r="K90" s="29"/>
       <c r="L90" s="31"/>
@@ -6704,30 +6704,32 @@
       <c r="N90" s="33"/>
       <c r="P90" s="29"/>
       <c r="Q90" s="32"/>
-      <c r="R90" s="40"/>
+      <c r="R90" s="34" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="91" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A91" s="35" t="s">
-        <v>1062</v>
+      <c r="A91" s="65" t="s">
+        <v>1060</v>
       </c>
       <c r="B91" s="43" t="s">
-        <v>1071</v>
+        <v>1064</v>
       </c>
       <c r="C91" s="59" t="s">
         <v>20</v>
       </c>
       <c r="D91" s="21" t="s">
-        <v>1069</v>
+        <v>1079</v>
       </c>
       <c r="E91" s="43" t="s">
-        <v>1071</v>
+        <v>1080</v>
       </c>
       <c r="G91" s="29"/>
       <c r="H91" s="21" t="s">
-        <v>1069</v>
+        <v>1079</v>
       </c>
       <c r="I91" s="43" t="s">
-        <v>1070</v>
+        <v>1081</v>
       </c>
       <c r="K91" s="29"/>
       <c r="L91" s="31"/>
@@ -6739,26 +6741,26 @@
     </row>
     <row r="92" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A92" s="35" t="s">
-        <v>1072</v>
+        <v>1061</v>
       </c>
       <c r="B92" s="43" t="s">
-        <v>1074</v>
+        <v>1065</v>
       </c>
       <c r="C92" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D92" s="66" t="s">
-        <v>1075</v>
+      <c r="D92" s="21" t="s">
+        <v>1063</v>
       </c>
       <c r="E92" s="43" t="s">
-        <v>1074</v>
+        <v>1064</v>
       </c>
       <c r="G92" s="29"/>
-      <c r="H92" s="66" t="s">
-        <v>1075</v>
+      <c r="H92" s="21" t="s">
+        <v>1063</v>
       </c>
       <c r="I92" s="43" t="s">
-        <v>1073</v>
+        <v>1082</v>
       </c>
       <c r="K92" s="29"/>
       <c r="L92" s="31"/>
@@ -6769,14 +6771,28 @@
       <c r="R92" s="40"/>
     </row>
     <row r="93" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A93" s="35"/>
-      <c r="B93" s="35"/>
-      <c r="C93" s="59"/>
-      <c r="D93" s="21"/>
-      <c r="E93" s="43"/>
+      <c r="A93" s="35" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B93" s="43" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C93" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="D93" s="21" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E93" s="43" t="s">
+        <v>1068</v>
+      </c>
       <c r="G93" s="29"/>
-      <c r="H93" s="21"/>
-      <c r="I93" s="43"/>
+      <c r="H93" s="21" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I93" s="43" t="s">
+        <v>1067</v>
+      </c>
       <c r="K93" s="29"/>
       <c r="L93" s="31"/>
       <c r="M93" s="29"/>
@@ -6786,13 +6802,28 @@
       <c r="R93" s="40"/>
     </row>
     <row r="94" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A94" s="27"/>
-      <c r="B94" s="39"/>
-      <c r="D94" s="31"/>
-      <c r="E94" s="33"/>
+      <c r="A94" s="35" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B94" s="43" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C94" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="D94" s="66" t="s">
+        <v>1072</v>
+      </c>
+      <c r="E94" s="43" t="s">
+        <v>1071</v>
+      </c>
       <c r="G94" s="29"/>
-      <c r="H94" s="31"/>
-      <c r="I94" s="33"/>
+      <c r="H94" s="66" t="s">
+        <v>1072</v>
+      </c>
+      <c r="I94" s="43" t="s">
+        <v>1070</v>
+      </c>
       <c r="K94" s="29"/>
       <c r="L94" s="31"/>
       <c r="M94" s="29"/>
@@ -6802,93 +6833,60 @@
       <c r="R94" s="40"/>
     </row>
     <row r="95" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A95" s="19" t="s">
-        <v>833</v>
-      </c>
-      <c r="B95" s="43" t="s">
-        <v>835</v>
-      </c>
-      <c r="C95" s="21" t="s">
-        <v>834</v>
-      </c>
-      <c r="D95" s="23" t="s">
-        <v>834</v>
-      </c>
-      <c r="E95" s="26" t="s">
-        <v>835</v>
-      </c>
+      <c r="A95" s="35"/>
+      <c r="B95" s="35"/>
+      <c r="C95" s="59"/>
+      <c r="D95" s="21"/>
+      <c r="E95" s="43"/>
       <c r="G95" s="29"/>
-      <c r="H95" s="23" t="s">
-        <v>834</v>
-      </c>
-      <c r="I95" s="26" t="s">
-        <v>836</v>
-      </c>
+      <c r="H95" s="21"/>
+      <c r="I95" s="43"/>
       <c r="K95" s="29"/>
       <c r="L95" s="31"/>
       <c r="M95" s="29"/>
       <c r="N95" s="33"/>
       <c r="P95" s="29"/>
       <c r="Q95" s="32"/>
-      <c r="R95" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R95" s="40"/>
     </row>
     <row r="96" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A96" s="19" t="s">
-        <v>837</v>
-      </c>
-      <c r="B96" s="43" t="s">
-        <v>839</v>
-      </c>
-      <c r="C96" s="21" t="s">
-        <v>838</v>
-      </c>
-      <c r="D96" s="23" t="s">
-        <v>838</v>
-      </c>
-      <c r="E96" s="26" t="s">
-        <v>839</v>
-      </c>
+      <c r="A96" s="27"/>
+      <c r="B96" s="39"/>
+      <c r="D96" s="31"/>
+      <c r="E96" s="33"/>
       <c r="G96" s="29"/>
-      <c r="H96" s="23" t="s">
-        <v>838</v>
-      </c>
-      <c r="I96" s="26" t="s">
-        <v>840</v>
-      </c>
+      <c r="H96" s="31"/>
+      <c r="I96" s="33"/>
       <c r="K96" s="29"/>
       <c r="L96" s="31"/>
       <c r="M96" s="29"/>
       <c r="N96" s="33"/>
       <c r="P96" s="29"/>
       <c r="Q96" s="32"/>
-      <c r="R96" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R96" s="40"/>
     </row>
     <row r="97" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A97" s="19" t="s">
-        <v>841</v>
+        <v>833</v>
       </c>
       <c r="B97" s="43" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
       <c r="C97" s="21" t="s">
-        <v>20</v>
+        <v>834</v>
       </c>
       <c r="D97" s="23" t="s">
-        <v>842</v>
+        <v>834</v>
       </c>
       <c r="E97" s="26" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
       <c r="G97" s="29"/>
-      <c r="H97" s="42" t="s">
-        <v>842</v>
+      <c r="H97" s="23" t="s">
+        <v>834</v>
       </c>
       <c r="I97" s="26" t="s">
-        <v>844</v>
+        <v>836</v>
       </c>
       <c r="K97" s="29"/>
       <c r="L97" s="31"/>
@@ -6902,26 +6900,26 @@
     </row>
     <row r="98" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A98" s="19" t="s">
-        <v>845</v>
+        <v>837</v>
       </c>
       <c r="B98" s="43" t="s">
-        <v>847</v>
+        <v>839</v>
       </c>
       <c r="C98" s="21" t="s">
-        <v>20</v>
+        <v>838</v>
       </c>
       <c r="D98" s="23" t="s">
-        <v>846</v>
+        <v>838</v>
       </c>
       <c r="E98" s="26" t="s">
-        <v>847</v>
+        <v>839</v>
       </c>
       <c r="G98" s="29"/>
-      <c r="H98" s="42" t="s">
-        <v>846</v>
+      <c r="H98" s="23" t="s">
+        <v>838</v>
       </c>
       <c r="I98" s="26" t="s">
-        <v>848</v>
+        <v>840</v>
       </c>
       <c r="K98" s="29"/>
       <c r="L98" s="31"/>
@@ -6929,32 +6927,32 @@
       <c r="N98" s="33"/>
       <c r="P98" s="29"/>
       <c r="Q98" s="32"/>
-      <c r="R98" s="34" t="s">
-        <v>849</v>
+      <c r="R98" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A99" s="19" t="s">
-        <v>850</v>
+        <v>841</v>
       </c>
       <c r="B99" s="43" t="s">
-        <v>852</v>
+        <v>843</v>
       </c>
       <c r="C99" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D99" s="23" t="s">
-        <v>851</v>
+        <v>842</v>
       </c>
       <c r="E99" s="26" t="s">
-        <v>852</v>
+        <v>843</v>
       </c>
       <c r="G99" s="29"/>
       <c r="H99" s="42" t="s">
-        <v>851</v>
+        <v>842</v>
       </c>
       <c r="I99" s="26" t="s">
-        <v>853</v>
+        <v>844</v>
       </c>
       <c r="K99" s="29"/>
       <c r="L99" s="31"/>
@@ -6967,43 +6965,60 @@
       </c>
     </row>
     <row r="100" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A100" s="27"/>
-      <c r="B100" s="39"/>
-      <c r="D100" s="31"/>
-      <c r="E100" s="33"/>
+      <c r="A100" s="19" t="s">
+        <v>845</v>
+      </c>
+      <c r="B100" s="43" t="s">
+        <v>847</v>
+      </c>
+      <c r="C100" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D100" s="23" t="s">
+        <v>846</v>
+      </c>
+      <c r="E100" s="26" t="s">
+        <v>847</v>
+      </c>
       <c r="G100" s="29"/>
-      <c r="H100" s="31"/>
-      <c r="I100" s="33"/>
+      <c r="H100" s="42" t="s">
+        <v>846</v>
+      </c>
+      <c r="I100" s="26" t="s">
+        <v>848</v>
+      </c>
       <c r="K100" s="29"/>
       <c r="L100" s="31"/>
       <c r="M100" s="29"/>
       <c r="N100" s="33"/>
       <c r="P100" s="29"/>
       <c r="Q100" s="32"/>
-      <c r="R100" s="34"/>
+      <c r="R100" s="34" t="s">
+        <v>849</v>
+      </c>
     </row>
     <row r="101" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A101" s="19" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="B101" s="43" t="s">
-        <v>857</v>
+        <v>852</v>
       </c>
       <c r="C101" s="21" t="s">
-        <v>855</v>
+        <v>20</v>
       </c>
       <c r="D101" s="23" t="s">
-        <v>20</v>
+        <v>851</v>
       </c>
       <c r="E101" s="26" t="s">
-        <v>20</v>
+        <v>852</v>
       </c>
       <c r="G101" s="29"/>
-      <c r="H101" s="23" t="s">
-        <v>856</v>
+      <c r="H101" s="42" t="s">
+        <v>851</v>
       </c>
       <c r="I101" s="26" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="K101" s="29"/>
       <c r="L101" s="31"/>
@@ -7011,14 +7026,13 @@
       <c r="N101" s="33"/>
       <c r="P101" s="29"/>
       <c r="Q101" s="32"/>
-      <c r="R101" s="34" t="s">
-        <v>849</v>
+      <c r="R101" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A102" s="19"/>
+      <c r="A102" s="27"/>
       <c r="B102" s="39"/>
-      <c r="C102" s="21"/>
       <c r="D102" s="31"/>
       <c r="E102" s="33"/>
       <c r="G102" s="29"/>
@@ -7030,30 +7044,30 @@
       <c r="N102" s="33"/>
       <c r="P102" s="29"/>
       <c r="Q102" s="32"/>
-      <c r="R102" s="40"/>
+      <c r="R102" s="34"/>
     </row>
     <row r="103" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A103" s="19" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="B103" s="43" t="s">
-        <v>860</v>
-      </c>
-      <c r="C103" s="19" t="s">
-        <v>859</v>
-      </c>
-      <c r="D103" s="21" t="s">
-        <v>859</v>
+        <v>857</v>
+      </c>
+      <c r="C103" s="21" t="s">
+        <v>855</v>
+      </c>
+      <c r="D103" s="23" t="s">
+        <v>20</v>
       </c>
       <c r="E103" s="26" t="s">
-        <v>860</v>
-      </c>
-      <c r="G103" s="33"/>
-      <c r="H103" s="21" t="s">
-        <v>859</v>
+        <v>20</v>
+      </c>
+      <c r="G103" s="29"/>
+      <c r="H103" s="23" t="s">
+        <v>856</v>
       </c>
       <c r="I103" s="26" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="K103" s="29"/>
       <c r="L103" s="31"/>
@@ -7061,81 +7075,82 @@
       <c r="N103" s="33"/>
       <c r="P103" s="29"/>
       <c r="Q103" s="32"/>
-      <c r="R103" s="34" t="b">
-        <v>1</v>
+      <c r="R103" s="34" t="s">
+        <v>849</v>
       </c>
     </row>
     <row r="104" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A104" s="19" t="s">
-        <v>862</v>
-      </c>
-      <c r="B104" s="43" t="s">
-        <v>864</v>
-      </c>
-      <c r="C104" s="21" t="s">
-        <v>863</v>
-      </c>
-      <c r="D104" s="23" t="s">
-        <v>863</v>
-      </c>
-      <c r="E104" s="26" t="s">
-        <v>864</v>
-      </c>
+      <c r="A104" s="19"/>
+      <c r="B104" s="39"/>
+      <c r="C104" s="21"/>
+      <c r="D104" s="31"/>
+      <c r="E104" s="33"/>
       <c r="G104" s="29"/>
-      <c r="H104" s="23" t="s">
-        <v>863</v>
-      </c>
-      <c r="I104" s="26" t="s">
-        <v>865</v>
-      </c>
+      <c r="H104" s="31"/>
+      <c r="I104" s="33"/>
       <c r="K104" s="29"/>
       <c r="L104" s="31"/>
       <c r="M104" s="29"/>
       <c r="N104" s="33"/>
       <c r="P104" s="29"/>
       <c r="Q104" s="32"/>
-      <c r="R104" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R104" s="40"/>
     </row>
     <row r="105" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A105" s="27"/>
-      <c r="B105" s="39"/>
-      <c r="D105" s="31"/>
-      <c r="E105" s="33"/>
-      <c r="G105" s="29"/>
-      <c r="H105" s="31"/>
-      <c r="I105" s="33"/>
+      <c r="A105" s="19" t="s">
+        <v>858</v>
+      </c>
+      <c r="B105" s="43" t="s">
+        <v>860</v>
+      </c>
+      <c r="C105" s="19" t="s">
+        <v>859</v>
+      </c>
+      <c r="D105" s="21" t="s">
+        <v>859</v>
+      </c>
+      <c r="E105" s="26" t="s">
+        <v>860</v>
+      </c>
+      <c r="G105" s="33"/>
+      <c r="H105" s="21" t="s">
+        <v>859</v>
+      </c>
+      <c r="I105" s="26" t="s">
+        <v>861</v>
+      </c>
       <c r="K105" s="29"/>
       <c r="L105" s="31"/>
       <c r="M105" s="29"/>
       <c r="N105" s="33"/>
       <c r="P105" s="29"/>
       <c r="Q105" s="32"/>
-      <c r="R105" s="40"/>
+      <c r="R105" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="106" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A106" s="19" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="B106" s="43" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="C106" s="21" t="s">
-        <v>20</v>
+        <v>863</v>
       </c>
       <c r="D106" s="23" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="E106" s="26" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="G106" s="29"/>
       <c r="H106" s="23" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="I106" s="26" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="K106" s="29"/>
       <c r="L106" s="31"/>
@@ -7143,65 +7158,48 @@
       <c r="N106" s="33"/>
       <c r="P106" s="29"/>
       <c r="Q106" s="32"/>
-      <c r="R106" s="34" t="s">
-        <v>33</v>
+      <c r="R106" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A107" s="19" t="s">
-        <v>870</v>
-      </c>
-      <c r="B107" s="43" t="s">
-        <v>872</v>
-      </c>
-      <c r="C107" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D107" s="23" t="s">
-        <v>871</v>
-      </c>
-      <c r="E107" s="26" t="s">
-        <v>872</v>
-      </c>
+      <c r="A107" s="27"/>
+      <c r="B107" s="39"/>
+      <c r="D107" s="31"/>
+      <c r="E107" s="33"/>
       <c r="G107" s="29"/>
-      <c r="H107" s="23" t="s">
-        <v>871</v>
-      </c>
-      <c r="I107" s="26" t="s">
-        <v>873</v>
-      </c>
+      <c r="H107" s="31"/>
+      <c r="I107" s="33"/>
       <c r="K107" s="29"/>
       <c r="L107" s="31"/>
       <c r="M107" s="29"/>
       <c r="N107" s="33"/>
       <c r="P107" s="29"/>
       <c r="Q107" s="32"/>
-      <c r="R107" s="34" t="s">
-        <v>33</v>
-      </c>
+      <c r="R107" s="40"/>
     </row>
     <row r="108" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A108" s="19" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="B108" s="43" t="s">
-        <v>876</v>
+        <v>868</v>
       </c>
       <c r="C108" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D108" s="23" t="s">
-        <v>875</v>
+        <v>867</v>
       </c>
       <c r="E108" s="26" t="s">
-        <v>876</v>
+        <v>868</v>
       </c>
       <c r="G108" s="29"/>
       <c r="H108" s="23" t="s">
-        <v>875</v>
+        <v>867</v>
       </c>
       <c r="I108" s="26" t="s">
-        <v>877</v>
+        <v>869</v>
       </c>
       <c r="K108" s="29"/>
       <c r="L108" s="31"/>
@@ -7215,26 +7213,26 @@
     </row>
     <row r="109" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A109" s="19" t="s">
-        <v>878</v>
+        <v>870</v>
       </c>
       <c r="B109" s="43" t="s">
-        <v>880</v>
+        <v>872</v>
       </c>
       <c r="C109" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D109" s="23" t="s">
-        <v>879</v>
+        <v>871</v>
       </c>
       <c r="E109" s="26" t="s">
-        <v>880</v>
+        <v>872</v>
       </c>
       <c r="G109" s="29"/>
       <c r="H109" s="23" t="s">
-        <v>879</v>
+        <v>871</v>
       </c>
       <c r="I109" s="26" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="K109" s="29"/>
       <c r="L109" s="31"/>
@@ -7242,32 +7240,32 @@
       <c r="N109" s="33"/>
       <c r="P109" s="29"/>
       <c r="Q109" s="32"/>
-      <c r="R109" s="34" t="b">
-        <v>1</v>
+      <c r="R109" s="34" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="110" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A110" s="19" t="s">
-        <v>882</v>
+        <v>874</v>
       </c>
       <c r="B110" s="43" t="s">
-        <v>884</v>
+        <v>876</v>
       </c>
       <c r="C110" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D110" s="23" t="s">
-        <v>883</v>
+        <v>875</v>
       </c>
       <c r="E110" s="26" t="s">
-        <v>884</v>
+        <v>876</v>
       </c>
       <c r="G110" s="29"/>
       <c r="H110" s="23" t="s">
-        <v>883</v>
+        <v>875</v>
       </c>
       <c r="I110" s="26" t="s">
-        <v>885</v>
+        <v>877</v>
       </c>
       <c r="K110" s="29"/>
       <c r="L110" s="31"/>
@@ -7281,26 +7279,26 @@
     </row>
     <row r="111" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A111" s="19" t="s">
-        <v>886</v>
+        <v>878</v>
       </c>
       <c r="B111" s="43" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
       <c r="C111" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D111" s="23" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
       <c r="E111" s="26" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
       <c r="G111" s="29"/>
       <c r="H111" s="23" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
       <c r="I111" s="26" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="K111" s="29"/>
       <c r="L111" s="31"/>
@@ -7314,26 +7312,26 @@
     </row>
     <row r="112" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A112" s="19" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="B112" s="43" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="C112" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D112" s="23" t="s">
-        <v>891</v>
+        <v>883</v>
       </c>
       <c r="E112" s="26" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="G112" s="29"/>
       <c r="H112" s="23" t="s">
-        <v>891</v>
+        <v>883</v>
       </c>
       <c r="I112" s="26" t="s">
-        <v>893</v>
+        <v>885</v>
       </c>
       <c r="K112" s="29"/>
       <c r="L112" s="31"/>
@@ -7341,46 +7339,84 @@
       <c r="N112" s="33"/>
       <c r="P112" s="29"/>
       <c r="Q112" s="32"/>
-      <c r="R112" s="34" t="b">
-        <v>1</v>
+      <c r="R112" s="34" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="113" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A113" s="27"/>
-      <c r="B113" s="39"/>
-      <c r="D113" s="31"/>
-      <c r="E113" s="33"/>
+      <c r="A113" s="19" t="s">
+        <v>886</v>
+      </c>
+      <c r="B113" s="43" t="s">
+        <v>888</v>
+      </c>
+      <c r="C113" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D113" s="23" t="s">
+        <v>887</v>
+      </c>
+      <c r="E113" s="26" t="s">
+        <v>888</v>
+      </c>
       <c r="G113" s="29"/>
-      <c r="H113" s="31"/>
-      <c r="I113" s="33"/>
+      <c r="H113" s="23" t="s">
+        <v>887</v>
+      </c>
+      <c r="I113" s="26" t="s">
+        <v>889</v>
+      </c>
       <c r="K113" s="29"/>
       <c r="L113" s="31"/>
       <c r="M113" s="29"/>
       <c r="N113" s="33"/>
       <c r="P113" s="29"/>
       <c r="Q113" s="32"/>
-      <c r="R113" s="27"/>
+      <c r="R113" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="114" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A114" s="27"/>
-      <c r="B114" s="39"/>
-      <c r="D114" s="31"/>
-      <c r="E114" s="33"/>
+      <c r="A114" s="19" t="s">
+        <v>890</v>
+      </c>
+      <c r="B114" s="43" t="s">
+        <v>892</v>
+      </c>
+      <c r="C114" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D114" s="23" t="s">
+        <v>891</v>
+      </c>
+      <c r="E114" s="26" t="s">
+        <v>892</v>
+      </c>
       <c r="G114" s="29"/>
-      <c r="H114" s="31"/>
-      <c r="I114" s="33"/>
+      <c r="H114" s="23" t="s">
+        <v>891</v>
+      </c>
+      <c r="I114" s="26" t="s">
+        <v>893</v>
+      </c>
       <c r="K114" s="29"/>
       <c r="L114" s="31"/>
       <c r="M114" s="29"/>
       <c r="N114" s="33"/>
       <c r="P114" s="29"/>
       <c r="Q114" s="32"/>
-      <c r="R114" s="27"/>
+      <c r="R114" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="115" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A115" s="27"/>
+      <c r="A115" s="27" t="s">
+        <v>1073</v>
+      </c>
       <c r="B115" s="39"/>
-      <c r="D115" s="31"/>
+      <c r="D115" s="31" t="s">
+        <v>1074</v>
+      </c>
       <c r="E115" s="33"/>
       <c r="G115" s="29"/>
       <c r="H115" s="31"/>
@@ -22320,6 +22356,38 @@
       <c r="P1048" s="29"/>
       <c r="Q1048" s="32"/>
       <c r="R1048" s="27"/>
+    </row>
+    <row r="1049" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1049" s="27"/>
+      <c r="B1049" s="39"/>
+      <c r="D1049" s="31"/>
+      <c r="E1049" s="33"/>
+      <c r="G1049" s="29"/>
+      <c r="H1049" s="31"/>
+      <c r="I1049" s="33"/>
+      <c r="K1049" s="29"/>
+      <c r="L1049" s="31"/>
+      <c r="M1049" s="29"/>
+      <c r="N1049" s="33"/>
+      <c r="P1049" s="29"/>
+      <c r="Q1049" s="32"/>
+      <c r="R1049" s="27"/>
+    </row>
+    <row r="1050" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1050" s="27"/>
+      <c r="B1050" s="39"/>
+      <c r="D1050" s="31"/>
+      <c r="E1050" s="33"/>
+      <c r="G1050" s="29"/>
+      <c r="H1050" s="31"/>
+      <c r="I1050" s="33"/>
+      <c r="K1050" s="29"/>
+      <c r="L1050" s="31"/>
+      <c r="M1050" s="29"/>
+      <c r="N1050" s="33"/>
+      <c r="P1050" s="29"/>
+      <c r="Q1050" s="32"/>
+      <c r="R1050" s="27"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" gridLines="1"/>
@@ -58217,7 +58285,7 @@
   </sheetPr>
   <dimension ref="A1:AB1030"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
more terms added for pig flatmap
</commit_message>
<xml_diff>
--- a/flatmap_annotation.xlsx
+++ b/flatmap_annotation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9278"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Body organs" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1800" uniqueCount="1083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="1130">
   <si>
     <t>Power point identifier</t>
   </si>
@@ -3254,9 +3254,6 @@
     <t>respiratory_13</t>
   </si>
   <si>
-    <t>nasopharynx</t>
-  </si>
-  <si>
     <t>arytenoid cartilage</t>
   </si>
   <si>
@@ -3273,6 +3270,150 @@
   </si>
   <si>
     <t xml:space="preserve"> ILX:0724443 </t>
+  </si>
+  <si>
+    <t>digestive_22</t>
+  </si>
+  <si>
+    <t>digestive_23</t>
+  </si>
+  <si>
+    <t>centripetal coil of colon</t>
+  </si>
+  <si>
+    <t>centrifugal coil of colon</t>
+  </si>
+  <si>
+    <t>digestive_24</t>
+  </si>
+  <si>
+    <t>digestive_25</t>
+  </si>
+  <si>
+    <t>ileum</t>
+  </si>
+  <si>
+    <t>UBERON:0002116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0728151  </t>
+  </si>
+  <si>
+    <t>ILX:0724224</t>
+  </si>
+  <si>
+    <t>jejunum</t>
+  </si>
+  <si>
+    <t>UBERON:0002115</t>
+  </si>
+  <si>
+    <t>reproductive_6</t>
+  </si>
+  <si>
+    <t>uterine horn</t>
+  </si>
+  <si>
+    <t>digestive_26</t>
+  </si>
+  <si>
+    <t>reproductive_7</t>
+  </si>
+  <si>
+    <t>mesometrium</t>
+  </si>
+  <si>
+    <t>UBERON:0003885</t>
+  </si>
+  <si>
+    <t>ILX:0725842</t>
+  </si>
+  <si>
+    <t>digestive_27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oral cavity </t>
+  </si>
+  <si>
+    <t>UBERON:0000167</t>
+  </si>
+  <si>
+    <t>nasal cavity</t>
+  </si>
+  <si>
+    <t>UBERON:0001707</t>
+  </si>
+  <si>
+    <t>UBERON:0001740</t>
+  </si>
+  <si>
+    <t>ILX:0727499</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LX:0733861  </t>
+  </si>
+  <si>
+    <t>duodenum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0002114 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0726125 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0729168 </t>
+  </si>
+  <si>
+    <t>oral cavity</t>
+  </si>
+  <si>
+    <t>UBERON:0002247</t>
+  </si>
+  <si>
+    <t>ILX:0733238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0001723  </t>
+  </si>
+  <si>
+    <t>ILX:0111810</t>
+  </si>
+  <si>
+    <t>digestive_28</t>
+  </si>
+  <si>
+    <t>digestive_29</t>
+  </si>
+  <si>
+    <t>proximal</t>
+  </si>
+  <si>
+    <t>right colon</t>
+  </si>
+  <si>
+    <t>UBERON:0008972</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0733240 </t>
+  </si>
+  <si>
+    <t>digestive_30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0728767  </t>
+  </si>
+  <si>
+    <t>distal</t>
+  </si>
+  <si>
+    <t>left colon</t>
+  </si>
+  <si>
+    <t>UBERON:0008971</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0727523 </t>
   </si>
 </sst>
 </file>
@@ -3579,7 +3720,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3688,6 +3829,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3906,10 +4051,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB1050"/>
+  <dimension ref="A1:AB1060"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C63" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="H100" sqref="H100"/>
+    <sheetView topLeftCell="A94" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101:B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -6092,15 +6237,23 @@
       <c r="A71" s="44" t="s">
         <v>1075</v>
       </c>
-      <c r="B71" s="35"/>
+      <c r="B71" s="43" t="s">
+        <v>1105</v>
+      </c>
       <c r="C71" s="21"/>
-      <c r="D71" s="42" t="s">
-        <v>1076</v>
-      </c>
-      <c r="E71" s="43"/>
+      <c r="D71" s="67" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E71" s="43" t="s">
+        <v>1105</v>
+      </c>
       <c r="G71" s="29"/>
-      <c r="H71" s="42"/>
-      <c r="I71" s="43"/>
+      <c r="H71" s="67" t="s">
+        <v>1104</v>
+      </c>
+      <c r="I71" s="68" t="s">
+        <v>1107</v>
+      </c>
       <c r="K71" s="29"/>
       <c r="L71" s="31"/>
       <c r="M71" s="29"/>
@@ -6111,17 +6264,25 @@
     </row>
     <row r="72" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A72" s="35" t="s">
-        <v>1078</v>
-      </c>
-      <c r="B72" s="35"/>
+        <v>1077</v>
+      </c>
+      <c r="B72" s="43" t="s">
+        <v>1106</v>
+      </c>
       <c r="C72" s="21"/>
       <c r="D72" s="67" t="s">
-        <v>1077</v>
-      </c>
-      <c r="E72" s="43"/>
+        <v>1076</v>
+      </c>
+      <c r="E72" s="43" t="s">
+        <v>1106</v>
+      </c>
       <c r="G72" s="29"/>
-      <c r="H72" s="42"/>
-      <c r="I72" s="43"/>
+      <c r="H72" s="67" t="s">
+        <v>1076</v>
+      </c>
+      <c r="I72" s="68" t="s">
+        <v>1108</v>
+      </c>
       <c r="K72" s="29"/>
       <c r="L72" s="31"/>
       <c r="M72" s="29"/>
@@ -6719,17 +6880,17 @@
         <v>20</v>
       </c>
       <c r="D91" s="21" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E91" s="43" t="s">
         <v>1079</v>
-      </c>
-      <c r="E91" s="43" t="s">
-        <v>1080</v>
       </c>
       <c r="G91" s="29"/>
       <c r="H91" s="21" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="I91" s="43" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="K91" s="29"/>
       <c r="L91" s="31"/>
@@ -6760,7 +6921,7 @@
         <v>1063</v>
       </c>
       <c r="I92" s="43" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="K92" s="29"/>
       <c r="L92" s="31"/>
@@ -6833,13 +6994,17 @@
       <c r="R94" s="40"/>
     </row>
     <row r="95" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A95" s="35"/>
+      <c r="A95" s="35" t="s">
+        <v>1082</v>
+      </c>
       <c r="B95" s="35"/>
       <c r="C95" s="59"/>
-      <c r="D95" s="21"/>
+      <c r="D95" s="66" t="s">
+        <v>1084</v>
+      </c>
       <c r="E95" s="43"/>
       <c r="G95" s="29"/>
-      <c r="H95" s="21"/>
+      <c r="H95" s="66"/>
       <c r="I95" s="43"/>
       <c r="K95" s="29"/>
       <c r="L95" s="31"/>
@@ -6850,13 +7015,18 @@
       <c r="R95" s="40"/>
     </row>
     <row r="96" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A96" s="27"/>
-      <c r="B96" s="39"/>
-      <c r="D96" s="31"/>
-      <c r="E96" s="33"/>
+      <c r="A96" s="35" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B96" s="35"/>
+      <c r="C96" s="59"/>
+      <c r="D96" s="66" t="s">
+        <v>1085</v>
+      </c>
+      <c r="E96" s="43"/>
       <c r="G96" s="29"/>
-      <c r="H96" s="31"/>
-      <c r="I96" s="33"/>
+      <c r="H96" s="66"/>
+      <c r="I96" s="43"/>
       <c r="K96" s="29"/>
       <c r="L96" s="31"/>
       <c r="M96" s="29"/>
@@ -6866,27 +7036,25 @@
       <c r="R96" s="40"/>
     </row>
     <row r="97" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A97" s="19" t="s">
-        <v>833</v>
+      <c r="A97" s="35" t="s">
+        <v>1086</v>
       </c>
       <c r="B97" s="43" t="s">
-        <v>835</v>
-      </c>
-      <c r="C97" s="21" t="s">
-        <v>834</v>
-      </c>
-      <c r="D97" s="23" t="s">
-        <v>834</v>
-      </c>
-      <c r="E97" s="26" t="s">
-        <v>835</v>
+        <v>1089</v>
+      </c>
+      <c r="C97" s="59"/>
+      <c r="D97" s="66" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E97" s="43" t="s">
+        <v>1089</v>
       </c>
       <c r="G97" s="29"/>
-      <c r="H97" s="23" t="s">
-        <v>834</v>
-      </c>
-      <c r="I97" s="26" t="s">
-        <v>836</v>
+      <c r="H97" s="66" t="s">
+        <v>1088</v>
+      </c>
+      <c r="I97" s="43" t="s">
+        <v>1090</v>
       </c>
       <c r="K97" s="29"/>
       <c r="L97" s="31"/>
@@ -6894,32 +7062,28 @@
       <c r="N97" s="33"/>
       <c r="P97" s="29"/>
       <c r="Q97" s="32"/>
-      <c r="R97" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R97" s="40"/>
     </row>
     <row r="98" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A98" s="19" t="s">
-        <v>837</v>
+      <c r="A98" s="35" t="s">
+        <v>1087</v>
       </c>
       <c r="B98" s="43" t="s">
-        <v>839</v>
-      </c>
-      <c r="C98" s="21" t="s">
-        <v>838</v>
-      </c>
-      <c r="D98" s="23" t="s">
-        <v>838</v>
-      </c>
-      <c r="E98" s="26" t="s">
-        <v>839</v>
+        <v>1093</v>
+      </c>
+      <c r="C98" s="59"/>
+      <c r="D98" s="21" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E98" s="43" t="s">
+        <v>1093</v>
       </c>
       <c r="G98" s="29"/>
-      <c r="H98" s="23" t="s">
-        <v>838</v>
-      </c>
-      <c r="I98" s="26" t="s">
-        <v>840</v>
+      <c r="H98" s="21" t="s">
+        <v>1092</v>
+      </c>
+      <c r="I98" s="43" t="s">
+        <v>1091</v>
       </c>
       <c r="K98" s="29"/>
       <c r="L98" s="31"/>
@@ -6927,32 +7091,28 @@
       <c r="N98" s="33"/>
       <c r="P98" s="29"/>
       <c r="Q98" s="32"/>
-      <c r="R98" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R98" s="40"/>
     </row>
     <row r="99" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A99" s="19" t="s">
-        <v>841</v>
+      <c r="A99" s="35" t="s">
+        <v>1096</v>
       </c>
       <c r="B99" s="43" t="s">
-        <v>843</v>
-      </c>
-      <c r="C99" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D99" s="23" t="s">
-        <v>842</v>
-      </c>
-      <c r="E99" s="26" t="s">
-        <v>843</v>
+        <v>1110</v>
+      </c>
+      <c r="C99" s="59"/>
+      <c r="D99" s="66" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E99" s="43" t="s">
+        <v>1110</v>
       </c>
       <c r="G99" s="29"/>
-      <c r="H99" s="42" t="s">
-        <v>842</v>
-      </c>
-      <c r="I99" s="26" t="s">
-        <v>844</v>
+      <c r="H99" s="66" t="s">
+        <v>1109</v>
+      </c>
+      <c r="I99" s="68" t="s">
+        <v>1111</v>
       </c>
       <c r="K99" s="29"/>
       <c r="L99" s="31"/>
@@ -6960,32 +7120,28 @@
       <c r="N99" s="33"/>
       <c r="P99" s="29"/>
       <c r="Q99" s="32"/>
-      <c r="R99" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R99" s="40"/>
     </row>
     <row r="100" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A100" s="19" t="s">
-        <v>845</v>
+      <c r="A100" s="35" t="s">
+        <v>1101</v>
       </c>
       <c r="B100" s="43" t="s">
-        <v>847</v>
-      </c>
-      <c r="C100" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D100" s="23" t="s">
-        <v>846</v>
-      </c>
-      <c r="E100" s="26" t="s">
-        <v>847</v>
+        <v>1103</v>
+      </c>
+      <c r="C100" s="59"/>
+      <c r="D100" s="66" t="s">
+        <v>1102</v>
+      </c>
+      <c r="E100" s="43" t="s">
+        <v>1103</v>
       </c>
       <c r="G100" s="29"/>
-      <c r="H100" s="42" t="s">
-        <v>846</v>
-      </c>
-      <c r="I100" s="26" t="s">
-        <v>848</v>
+      <c r="H100" s="66" t="s">
+        <v>1113</v>
+      </c>
+      <c r="I100" s="68" t="s">
+        <v>1112</v>
       </c>
       <c r="K100" s="29"/>
       <c r="L100" s="31"/>
@@ -6993,32 +7149,30 @@
       <c r="N100" s="33"/>
       <c r="P100" s="29"/>
       <c r="Q100" s="32"/>
-      <c r="R100" s="34" t="s">
-        <v>849</v>
-      </c>
+      <c r="R100" s="40"/>
     </row>
     <row r="101" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A101" s="19" t="s">
-        <v>850</v>
-      </c>
-      <c r="B101" s="43" t="s">
-        <v>852</v>
-      </c>
-      <c r="C101" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D101" s="23" t="s">
-        <v>851</v>
-      </c>
-      <c r="E101" s="26" t="s">
-        <v>852</v>
+      <c r="A101" s="35" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B101" s="68" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C101" s="71" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D101" s="66" t="s">
+        <v>1121</v>
+      </c>
+      <c r="E101" s="68" t="s">
+        <v>1122</v>
       </c>
       <c r="G101" s="29"/>
-      <c r="H101" s="42" t="s">
-        <v>851</v>
-      </c>
-      <c r="I101" s="26" t="s">
-        <v>853</v>
+      <c r="H101" s="66" t="s">
+        <v>1121</v>
+      </c>
+      <c r="I101" s="68" t="s">
+        <v>1123</v>
       </c>
       <c r="K101" s="29"/>
       <c r="L101" s="31"/>
@@ -7026,48 +7180,59 @@
       <c r="N101" s="33"/>
       <c r="P101" s="29"/>
       <c r="Q101" s="32"/>
-      <c r="R101" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R101" s="40"/>
     </row>
     <row r="102" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A102" s="27"/>
-      <c r="B102" s="39"/>
-      <c r="D102" s="31"/>
-      <c r="E102" s="33"/>
+      <c r="A102" s="35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B102" s="68" t="s">
+        <v>821</v>
+      </c>
+      <c r="C102" s="59"/>
+      <c r="D102" s="66" t="s">
+        <v>820</v>
+      </c>
+      <c r="E102" s="68" t="s">
+        <v>821</v>
+      </c>
       <c r="G102" s="29"/>
-      <c r="H102" s="31"/>
-      <c r="I102" s="33"/>
+      <c r="H102" s="66" t="s">
+        <v>820</v>
+      </c>
+      <c r="I102" s="68" t="s">
+        <v>1125</v>
+      </c>
       <c r="K102" s="29"/>
       <c r="L102" s="31"/>
       <c r="M102" s="29"/>
       <c r="N102" s="33"/>
       <c r="P102" s="29"/>
       <c r="Q102" s="32"/>
-      <c r="R102" s="34"/>
+      <c r="R102" s="40"/>
     </row>
     <row r="103" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A103" s="19" t="s">
-        <v>854</v>
-      </c>
-      <c r="B103" s="43" t="s">
-        <v>857</v>
-      </c>
-      <c r="C103" s="21" t="s">
-        <v>855</v>
-      </c>
-      <c r="D103" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E103" s="26" t="s">
-        <v>20</v>
+      <c r="A103" s="35" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B103" s="68" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C103" s="71" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D103" s="66" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E103" s="68" t="s">
+        <v>1128</v>
       </c>
       <c r="G103" s="29"/>
-      <c r="H103" s="23" t="s">
-        <v>856</v>
-      </c>
-      <c r="I103" s="26" t="s">
-        <v>857</v>
+      <c r="H103" s="66" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I103" s="68" t="s">
+        <v>1129</v>
       </c>
       <c r="K103" s="29"/>
       <c r="L103" s="31"/>
@@ -7075,14 +7240,11 @@
       <c r="N103" s="33"/>
       <c r="P103" s="29"/>
       <c r="Q103" s="32"/>
-      <c r="R103" s="34" t="s">
-        <v>849</v>
-      </c>
+      <c r="R103" s="40"/>
     </row>
     <row r="104" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A104" s="19"/>
+      <c r="A104" s="27"/>
       <c r="B104" s="39"/>
-      <c r="C104" s="21"/>
       <c r="D104" s="31"/>
       <c r="E104" s="33"/>
       <c r="G104" s="29"/>
@@ -7098,26 +7260,26 @@
     </row>
     <row r="105" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A105" s="19" t="s">
-        <v>858</v>
+        <v>833</v>
       </c>
       <c r="B105" s="43" t="s">
-        <v>860</v>
-      </c>
-      <c r="C105" s="19" t="s">
-        <v>859</v>
-      </c>
-      <c r="D105" s="21" t="s">
-        <v>859</v>
+        <v>835</v>
+      </c>
+      <c r="C105" s="21" t="s">
+        <v>834</v>
+      </c>
+      <c r="D105" s="23" t="s">
+        <v>834</v>
       </c>
       <c r="E105" s="26" t="s">
-        <v>860</v>
-      </c>
-      <c r="G105" s="33"/>
-      <c r="H105" s="21" t="s">
-        <v>859</v>
+        <v>835</v>
+      </c>
+      <c r="G105" s="29"/>
+      <c r="H105" s="23" t="s">
+        <v>834</v>
       </c>
       <c r="I105" s="26" t="s">
-        <v>861</v>
+        <v>836</v>
       </c>
       <c r="K105" s="29"/>
       <c r="L105" s="31"/>
@@ -7131,26 +7293,26 @@
     </row>
     <row r="106" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A106" s="19" t="s">
-        <v>862</v>
+        <v>837</v>
       </c>
       <c r="B106" s="43" t="s">
-        <v>864</v>
+        <v>839</v>
       </c>
       <c r="C106" s="21" t="s">
-        <v>863</v>
+        <v>838</v>
       </c>
       <c r="D106" s="23" t="s">
-        <v>863</v>
+        <v>838</v>
       </c>
       <c r="E106" s="26" t="s">
-        <v>864</v>
+        <v>839</v>
       </c>
       <c r="G106" s="29"/>
       <c r="H106" s="23" t="s">
-        <v>863</v>
+        <v>838</v>
       </c>
       <c r="I106" s="26" t="s">
-        <v>865</v>
+        <v>840</v>
       </c>
       <c r="K106" s="29"/>
       <c r="L106" s="31"/>
@@ -7163,43 +7325,60 @@
       </c>
     </row>
     <row r="107" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A107" s="27"/>
-      <c r="B107" s="39"/>
-      <c r="D107" s="31"/>
-      <c r="E107" s="33"/>
+      <c r="A107" s="19" t="s">
+        <v>841</v>
+      </c>
+      <c r="B107" s="43" t="s">
+        <v>843</v>
+      </c>
+      <c r="C107" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D107" s="23" t="s">
+        <v>842</v>
+      </c>
+      <c r="E107" s="26" t="s">
+        <v>843</v>
+      </c>
       <c r="G107" s="29"/>
-      <c r="H107" s="31"/>
-      <c r="I107" s="33"/>
+      <c r="H107" s="42" t="s">
+        <v>842</v>
+      </c>
+      <c r="I107" s="26" t="s">
+        <v>844</v>
+      </c>
       <c r="K107" s="29"/>
       <c r="L107" s="31"/>
       <c r="M107" s="29"/>
       <c r="N107" s="33"/>
       <c r="P107" s="29"/>
       <c r="Q107" s="32"/>
-      <c r="R107" s="40"/>
+      <c r="R107" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="108" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A108" s="19" t="s">
-        <v>866</v>
+        <v>845</v>
       </c>
       <c r="B108" s="43" t="s">
-        <v>868</v>
+        <v>847</v>
       </c>
       <c r="C108" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D108" s="23" t="s">
-        <v>867</v>
+        <v>846</v>
       </c>
       <c r="E108" s="26" t="s">
-        <v>868</v>
+        <v>847</v>
       </c>
       <c r="G108" s="29"/>
-      <c r="H108" s="23" t="s">
-        <v>867</v>
+      <c r="H108" s="42" t="s">
+        <v>846</v>
       </c>
       <c r="I108" s="26" t="s">
-        <v>869</v>
+        <v>848</v>
       </c>
       <c r="K108" s="29"/>
       <c r="L108" s="31"/>
@@ -7208,31 +7387,31 @@
       <c r="P108" s="29"/>
       <c r="Q108" s="32"/>
       <c r="R108" s="34" t="s">
-        <v>33</v>
+        <v>849</v>
       </c>
     </row>
     <row r="109" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A109" s="19" t="s">
-        <v>870</v>
+        <v>850</v>
       </c>
       <c r="B109" s="43" t="s">
-        <v>872</v>
+        <v>852</v>
       </c>
       <c r="C109" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D109" s="23" t="s">
-        <v>871</v>
+        <v>851</v>
       </c>
       <c r="E109" s="26" t="s">
-        <v>872</v>
+        <v>852</v>
       </c>
       <c r="G109" s="29"/>
-      <c r="H109" s="23" t="s">
-        <v>871</v>
+      <c r="H109" s="42" t="s">
+        <v>851</v>
       </c>
       <c r="I109" s="26" t="s">
-        <v>873</v>
+        <v>853</v>
       </c>
       <c r="K109" s="29"/>
       <c r="L109" s="31"/>
@@ -7240,32 +7419,30 @@
       <c r="N109" s="33"/>
       <c r="P109" s="29"/>
       <c r="Q109" s="32"/>
-      <c r="R109" s="34" t="s">
-        <v>33</v>
+      <c r="R109" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A110" s="19" t="s">
-        <v>874</v>
-      </c>
-      <c r="B110" s="43" t="s">
-        <v>876</v>
-      </c>
-      <c r="C110" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D110" s="23" t="s">
-        <v>875</v>
-      </c>
-      <c r="E110" s="26" t="s">
-        <v>876</v>
+      <c r="A110" s="35" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B110" s="68" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C110" s="21"/>
+      <c r="D110" s="67" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E110" s="68" t="s">
+        <v>1114</v>
       </c>
       <c r="G110" s="29"/>
-      <c r="H110" s="23" t="s">
-        <v>875</v>
-      </c>
-      <c r="I110" s="26" t="s">
-        <v>877</v>
+      <c r="H110" s="67" t="s">
+        <v>1095</v>
+      </c>
+      <c r="I110" s="43" t="s">
+        <v>1115</v>
       </c>
       <c r="K110" s="29"/>
       <c r="L110" s="31"/>
@@ -7273,32 +7450,28 @@
       <c r="N110" s="33"/>
       <c r="P110" s="29"/>
       <c r="Q110" s="32"/>
-      <c r="R110" s="34" t="s">
-        <v>33</v>
-      </c>
+      <c r="R110" s="40"/>
     </row>
     <row r="111" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A111" s="19" t="s">
-        <v>878</v>
+      <c r="A111" s="35" t="s">
+        <v>1097</v>
       </c>
       <c r="B111" s="43" t="s">
-        <v>880</v>
-      </c>
-      <c r="C111" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D111" s="23" t="s">
-        <v>879</v>
-      </c>
-      <c r="E111" s="26" t="s">
-        <v>880</v>
+        <v>1099</v>
+      </c>
+      <c r="C111" s="21"/>
+      <c r="D111" s="42" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E111" s="43" t="s">
+        <v>1099</v>
       </c>
       <c r="G111" s="29"/>
-      <c r="H111" s="23" t="s">
-        <v>879</v>
-      </c>
-      <c r="I111" s="26" t="s">
-        <v>881</v>
+      <c r="H111" s="42" t="s">
+        <v>1098</v>
+      </c>
+      <c r="I111" s="43" t="s">
+        <v>1100</v>
       </c>
       <c r="K111" s="29"/>
       <c r="L111" s="31"/>
@@ -7306,65 +7479,46 @@
       <c r="N111" s="33"/>
       <c r="P111" s="29"/>
       <c r="Q111" s="32"/>
-      <c r="R111" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R111" s="40"/>
     </row>
     <row r="112" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A112" s="19" t="s">
-        <v>882</v>
-      </c>
-      <c r="B112" s="43" t="s">
-        <v>884</v>
-      </c>
-      <c r="C112" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D112" s="23" t="s">
-        <v>883</v>
-      </c>
-      <c r="E112" s="26" t="s">
-        <v>884</v>
-      </c>
+      <c r="A112" s="27"/>
+      <c r="B112" s="39"/>
+      <c r="D112" s="31"/>
+      <c r="E112" s="33"/>
       <c r="G112" s="29"/>
-      <c r="H112" s="23" t="s">
-        <v>883</v>
-      </c>
-      <c r="I112" s="26" t="s">
-        <v>885</v>
-      </c>
+      <c r="H112" s="31"/>
+      <c r="I112" s="33"/>
       <c r="K112" s="29"/>
       <c r="L112" s="31"/>
       <c r="M112" s="29"/>
       <c r="N112" s="33"/>
       <c r="P112" s="29"/>
       <c r="Q112" s="32"/>
-      <c r="R112" s="34" t="s">
-        <v>33</v>
-      </c>
+      <c r="R112" s="34"/>
     </row>
     <row r="113" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A113" s="19" t="s">
-        <v>886</v>
+        <v>854</v>
       </c>
       <c r="B113" s="43" t="s">
-        <v>888</v>
+        <v>857</v>
       </c>
       <c r="C113" s="21" t="s">
+        <v>855</v>
+      </c>
+      <c r="D113" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D113" s="23" t="s">
-        <v>887</v>
-      </c>
       <c r="E113" s="26" t="s">
-        <v>888</v>
+        <v>20</v>
       </c>
       <c r="G113" s="29"/>
       <c r="H113" s="23" t="s">
-        <v>887</v>
+        <v>856</v>
       </c>
       <c r="I113" s="26" t="s">
-        <v>889</v>
+        <v>857</v>
       </c>
       <c r="K113" s="29"/>
       <c r="L113" s="31"/>
@@ -7372,78 +7526,92 @@
       <c r="N113" s="33"/>
       <c r="P113" s="29"/>
       <c r="Q113" s="32"/>
-      <c r="R113" s="34" t="b">
-        <v>1</v>
+      <c r="R113" s="34" t="s">
+        <v>849</v>
       </c>
     </row>
     <row r="114" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A114" s="19" t="s">
-        <v>890</v>
-      </c>
-      <c r="B114" s="43" t="s">
-        <v>892</v>
-      </c>
-      <c r="C114" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D114" s="23" t="s">
-        <v>891</v>
-      </c>
-      <c r="E114" s="26" t="s">
-        <v>892</v>
-      </c>
+      <c r="A114" s="19"/>
+      <c r="B114" s="39"/>
+      <c r="C114" s="21"/>
+      <c r="D114" s="31"/>
+      <c r="E114" s="33"/>
       <c r="G114" s="29"/>
-      <c r="H114" s="23" t="s">
-        <v>891</v>
-      </c>
-      <c r="I114" s="26" t="s">
-        <v>893</v>
-      </c>
+      <c r="H114" s="31"/>
+      <c r="I114" s="33"/>
       <c r="K114" s="29"/>
       <c r="L114" s="31"/>
       <c r="M114" s="29"/>
       <c r="N114" s="33"/>
       <c r="P114" s="29"/>
       <c r="Q114" s="32"/>
-      <c r="R114" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R114" s="40"/>
     </row>
     <row r="115" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A115" s="27" t="s">
-        <v>1073</v>
-      </c>
-      <c r="B115" s="39"/>
-      <c r="D115" s="31" t="s">
-        <v>1074</v>
-      </c>
-      <c r="E115" s="33"/>
-      <c r="G115" s="29"/>
-      <c r="H115" s="31"/>
-      <c r="I115" s="33"/>
+      <c r="A115" s="19" t="s">
+        <v>858</v>
+      </c>
+      <c r="B115" s="43" t="s">
+        <v>860</v>
+      </c>
+      <c r="C115" s="19" t="s">
+        <v>859</v>
+      </c>
+      <c r="D115" s="21" t="s">
+        <v>859</v>
+      </c>
+      <c r="E115" s="26" t="s">
+        <v>860</v>
+      </c>
+      <c r="G115" s="33"/>
+      <c r="H115" s="21" t="s">
+        <v>859</v>
+      </c>
+      <c r="I115" s="26" t="s">
+        <v>861</v>
+      </c>
       <c r="K115" s="29"/>
       <c r="L115" s="31"/>
       <c r="M115" s="29"/>
       <c r="N115" s="33"/>
       <c r="P115" s="29"/>
       <c r="Q115" s="32"/>
-      <c r="R115" s="27"/>
+      <c r="R115" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="116" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A116" s="27"/>
-      <c r="B116" s="39"/>
-      <c r="D116" s="31"/>
-      <c r="E116" s="33"/>
+      <c r="A116" s="19" t="s">
+        <v>862</v>
+      </c>
+      <c r="B116" s="43" t="s">
+        <v>864</v>
+      </c>
+      <c r="C116" s="21" t="s">
+        <v>863</v>
+      </c>
+      <c r="D116" s="23" t="s">
+        <v>863</v>
+      </c>
+      <c r="E116" s="26" t="s">
+        <v>864</v>
+      </c>
       <c r="G116" s="29"/>
-      <c r="H116" s="31"/>
-      <c r="I116" s="33"/>
+      <c r="H116" s="23" t="s">
+        <v>863</v>
+      </c>
+      <c r="I116" s="26" t="s">
+        <v>865</v>
+      </c>
       <c r="K116" s="29"/>
       <c r="L116" s="31"/>
       <c r="M116" s="29"/>
       <c r="N116" s="33"/>
       <c r="P116" s="29"/>
       <c r="Q116" s="32"/>
-      <c r="R116" s="27"/>
+      <c r="R116" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="117" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A117" s="27"/>
@@ -7459,128 +7627,259 @@
       <c r="N117" s="33"/>
       <c r="P117" s="29"/>
       <c r="Q117" s="32"/>
-      <c r="R117" s="27"/>
+      <c r="R117" s="40"/>
     </row>
     <row r="118" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A118" s="27"/>
-      <c r="B118" s="39"/>
-      <c r="D118" s="31"/>
-      <c r="E118" s="33"/>
+      <c r="A118" s="19" t="s">
+        <v>866</v>
+      </c>
+      <c r="B118" s="43" t="s">
+        <v>868</v>
+      </c>
+      <c r="C118" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D118" s="23" t="s">
+        <v>867</v>
+      </c>
+      <c r="E118" s="26" t="s">
+        <v>868</v>
+      </c>
       <c r="G118" s="29"/>
-      <c r="H118" s="31"/>
-      <c r="I118" s="33"/>
+      <c r="H118" s="23" t="s">
+        <v>867</v>
+      </c>
+      <c r="I118" s="26" t="s">
+        <v>869</v>
+      </c>
       <c r="K118" s="29"/>
       <c r="L118" s="31"/>
       <c r="M118" s="29"/>
       <c r="N118" s="33"/>
       <c r="P118" s="29"/>
       <c r="Q118" s="32"/>
-      <c r="R118" s="27"/>
+      <c r="R118" s="34" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="119" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A119" s="27"/>
-      <c r="B119" s="39"/>
-      <c r="D119" s="31"/>
-      <c r="E119" s="33"/>
+      <c r="A119" s="19" t="s">
+        <v>870</v>
+      </c>
+      <c r="B119" s="43" t="s">
+        <v>872</v>
+      </c>
+      <c r="C119" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D119" s="23" t="s">
+        <v>871</v>
+      </c>
+      <c r="E119" s="26" t="s">
+        <v>872</v>
+      </c>
       <c r="G119" s="29"/>
-      <c r="H119" s="31"/>
-      <c r="I119" s="33"/>
+      <c r="H119" s="23" t="s">
+        <v>871</v>
+      </c>
+      <c r="I119" s="26" t="s">
+        <v>873</v>
+      </c>
       <c r="K119" s="29"/>
       <c r="L119" s="31"/>
       <c r="M119" s="29"/>
       <c r="N119" s="33"/>
       <c r="P119" s="29"/>
       <c r="Q119" s="32"/>
-      <c r="R119" s="27"/>
+      <c r="R119" s="34" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="120" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A120" s="27"/>
-      <c r="B120" s="39"/>
-      <c r="D120" s="31"/>
-      <c r="E120" s="33"/>
+      <c r="A120" s="19" t="s">
+        <v>874</v>
+      </c>
+      <c r="B120" s="43" t="s">
+        <v>876</v>
+      </c>
+      <c r="C120" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D120" s="23" t="s">
+        <v>875</v>
+      </c>
+      <c r="E120" s="26" t="s">
+        <v>876</v>
+      </c>
       <c r="G120" s="29"/>
-      <c r="H120" s="31"/>
-      <c r="I120" s="33"/>
+      <c r="H120" s="23" t="s">
+        <v>875</v>
+      </c>
+      <c r="I120" s="26" t="s">
+        <v>877</v>
+      </c>
       <c r="K120" s="29"/>
       <c r="L120" s="31"/>
       <c r="M120" s="29"/>
       <c r="N120" s="33"/>
       <c r="P120" s="29"/>
       <c r="Q120" s="32"/>
-      <c r="R120" s="27"/>
+      <c r="R120" s="34" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="121" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A121" s="27"/>
-      <c r="B121" s="39"/>
-      <c r="D121" s="31"/>
-      <c r="E121" s="33"/>
+      <c r="A121" s="19" t="s">
+        <v>878</v>
+      </c>
+      <c r="B121" s="43" t="s">
+        <v>880</v>
+      </c>
+      <c r="C121" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D121" s="23" t="s">
+        <v>879</v>
+      </c>
+      <c r="E121" s="26" t="s">
+        <v>880</v>
+      </c>
       <c r="G121" s="29"/>
-      <c r="H121" s="31"/>
-      <c r="I121" s="33"/>
+      <c r="H121" s="23" t="s">
+        <v>879</v>
+      </c>
+      <c r="I121" s="26" t="s">
+        <v>881</v>
+      </c>
       <c r="K121" s="29"/>
       <c r="L121" s="31"/>
       <c r="M121" s="29"/>
       <c r="N121" s="33"/>
       <c r="P121" s="29"/>
       <c r="Q121" s="32"/>
-      <c r="R121" s="27"/>
+      <c r="R121" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="122" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A122" s="27"/>
-      <c r="B122" s="39"/>
-      <c r="D122" s="31"/>
-      <c r="E122" s="33"/>
+      <c r="A122" s="19" t="s">
+        <v>882</v>
+      </c>
+      <c r="B122" s="43" t="s">
+        <v>884</v>
+      </c>
+      <c r="C122" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D122" s="23" t="s">
+        <v>883</v>
+      </c>
+      <c r="E122" s="26" t="s">
+        <v>884</v>
+      </c>
       <c r="G122" s="29"/>
-      <c r="H122" s="31"/>
-      <c r="I122" s="33"/>
+      <c r="H122" s="23" t="s">
+        <v>883</v>
+      </c>
+      <c r="I122" s="26" t="s">
+        <v>885</v>
+      </c>
       <c r="K122" s="29"/>
       <c r="L122" s="31"/>
       <c r="M122" s="29"/>
       <c r="N122" s="33"/>
       <c r="P122" s="29"/>
       <c r="Q122" s="32"/>
-      <c r="R122" s="27"/>
+      <c r="R122" s="34" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="123" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A123" s="27"/>
-      <c r="B123" s="39"/>
-      <c r="D123" s="31"/>
-      <c r="E123" s="33"/>
+      <c r="A123" s="19" t="s">
+        <v>886</v>
+      </c>
+      <c r="B123" s="43" t="s">
+        <v>888</v>
+      </c>
+      <c r="C123" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D123" s="23" t="s">
+        <v>887</v>
+      </c>
+      <c r="E123" s="26" t="s">
+        <v>888</v>
+      </c>
       <c r="G123" s="29"/>
-      <c r="H123" s="31"/>
-      <c r="I123" s="33"/>
+      <c r="H123" s="23" t="s">
+        <v>887</v>
+      </c>
+      <c r="I123" s="26" t="s">
+        <v>889</v>
+      </c>
       <c r="K123" s="29"/>
       <c r="L123" s="31"/>
       <c r="M123" s="29"/>
       <c r="N123" s="33"/>
       <c r="P123" s="29"/>
       <c r="Q123" s="32"/>
-      <c r="R123" s="27"/>
+      <c r="R123" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="124" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A124" s="27"/>
-      <c r="B124" s="39"/>
-      <c r="D124" s="31"/>
-      <c r="E124" s="33"/>
+      <c r="A124" s="19" t="s">
+        <v>890</v>
+      </c>
+      <c r="B124" s="43" t="s">
+        <v>892</v>
+      </c>
+      <c r="C124" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D124" s="23" t="s">
+        <v>891</v>
+      </c>
+      <c r="E124" s="26" t="s">
+        <v>892</v>
+      </c>
       <c r="G124" s="29"/>
-      <c r="H124" s="31"/>
-      <c r="I124" s="33"/>
+      <c r="H124" s="23" t="s">
+        <v>891</v>
+      </c>
+      <c r="I124" s="26" t="s">
+        <v>893</v>
+      </c>
       <c r="K124" s="29"/>
       <c r="L124" s="31"/>
       <c r="M124" s="29"/>
       <c r="N124" s="33"/>
       <c r="P124" s="29"/>
       <c r="Q124" s="32"/>
-      <c r="R124" s="27"/>
+      <c r="R124" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="125" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A125" s="27"/>
-      <c r="B125" s="39"/>
-      <c r="D125" s="31"/>
-      <c r="E125" s="33"/>
+      <c r="A125" s="27" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B125" s="69" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D125" s="70" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E125" s="69" t="s">
+        <v>1116</v>
+      </c>
       <c r="G125" s="29"/>
-      <c r="H125" s="31"/>
-      <c r="I125" s="33"/>
+      <c r="H125" s="70" t="s">
+        <v>1074</v>
+      </c>
+      <c r="I125" s="69" t="s">
+        <v>1117</v>
+      </c>
       <c r="K125" s="29"/>
       <c r="L125" s="31"/>
       <c r="M125" s="29"/>
@@ -22388,6 +22687,166 @@
       <c r="P1050" s="29"/>
       <c r="Q1050" s="32"/>
       <c r="R1050" s="27"/>
+    </row>
+    <row r="1051" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1051" s="27"/>
+      <c r="B1051" s="39"/>
+      <c r="D1051" s="31"/>
+      <c r="E1051" s="33"/>
+      <c r="G1051" s="29"/>
+      <c r="H1051" s="31"/>
+      <c r="I1051" s="33"/>
+      <c r="K1051" s="29"/>
+      <c r="L1051" s="31"/>
+      <c r="M1051" s="29"/>
+      <c r="N1051" s="33"/>
+      <c r="P1051" s="29"/>
+      <c r="Q1051" s="32"/>
+      <c r="R1051" s="27"/>
+    </row>
+    <row r="1052" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1052" s="27"/>
+      <c r="B1052" s="39"/>
+      <c r="D1052" s="31"/>
+      <c r="E1052" s="33"/>
+      <c r="G1052" s="29"/>
+      <c r="H1052" s="31"/>
+      <c r="I1052" s="33"/>
+      <c r="K1052" s="29"/>
+      <c r="L1052" s="31"/>
+      <c r="M1052" s="29"/>
+      <c r="N1052" s="33"/>
+      <c r="P1052" s="29"/>
+      <c r="Q1052" s="32"/>
+      <c r="R1052" s="27"/>
+    </row>
+    <row r="1053" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1053" s="27"/>
+      <c r="B1053" s="39"/>
+      <c r="D1053" s="31"/>
+      <c r="E1053" s="33"/>
+      <c r="G1053" s="29"/>
+      <c r="H1053" s="31"/>
+      <c r="I1053" s="33"/>
+      <c r="K1053" s="29"/>
+      <c r="L1053" s="31"/>
+      <c r="M1053" s="29"/>
+      <c r="N1053" s="33"/>
+      <c r="P1053" s="29"/>
+      <c r="Q1053" s="32"/>
+      <c r="R1053" s="27"/>
+    </row>
+    <row r="1054" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1054" s="27"/>
+      <c r="B1054" s="39"/>
+      <c r="D1054" s="31"/>
+      <c r="E1054" s="33"/>
+      <c r="G1054" s="29"/>
+      <c r="H1054" s="31"/>
+      <c r="I1054" s="33"/>
+      <c r="K1054" s="29"/>
+      <c r="L1054" s="31"/>
+      <c r="M1054" s="29"/>
+      <c r="N1054" s="33"/>
+      <c r="P1054" s="29"/>
+      <c r="Q1054" s="32"/>
+      <c r="R1054" s="27"/>
+    </row>
+    <row r="1055" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1055" s="27"/>
+      <c r="B1055" s="39"/>
+      <c r="D1055" s="31"/>
+      <c r="E1055" s="33"/>
+      <c r="G1055" s="29"/>
+      <c r="H1055" s="31"/>
+      <c r="I1055" s="33"/>
+      <c r="K1055" s="29"/>
+      <c r="L1055" s="31"/>
+      <c r="M1055" s="29"/>
+      <c r="N1055" s="33"/>
+      <c r="P1055" s="29"/>
+      <c r="Q1055" s="32"/>
+      <c r="R1055" s="27"/>
+    </row>
+    <row r="1056" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1056" s="27"/>
+      <c r="B1056" s="39"/>
+      <c r="D1056" s="31"/>
+      <c r="E1056" s="33"/>
+      <c r="G1056" s="29"/>
+      <c r="H1056" s="31"/>
+      <c r="I1056" s="33"/>
+      <c r="K1056" s="29"/>
+      <c r="L1056" s="31"/>
+      <c r="M1056" s="29"/>
+      <c r="N1056" s="33"/>
+      <c r="P1056" s="29"/>
+      <c r="Q1056" s="32"/>
+      <c r="R1056" s="27"/>
+    </row>
+    <row r="1057" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1057" s="27"/>
+      <c r="B1057" s="39"/>
+      <c r="D1057" s="31"/>
+      <c r="E1057" s="33"/>
+      <c r="G1057" s="29"/>
+      <c r="H1057" s="31"/>
+      <c r="I1057" s="33"/>
+      <c r="K1057" s="29"/>
+      <c r="L1057" s="31"/>
+      <c r="M1057" s="29"/>
+      <c r="N1057" s="33"/>
+      <c r="P1057" s="29"/>
+      <c r="Q1057" s="32"/>
+      <c r="R1057" s="27"/>
+    </row>
+    <row r="1058" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1058" s="27"/>
+      <c r="B1058" s="39"/>
+      <c r="D1058" s="31"/>
+      <c r="E1058" s="33"/>
+      <c r="G1058" s="29"/>
+      <c r="H1058" s="31"/>
+      <c r="I1058" s="33"/>
+      <c r="K1058" s="29"/>
+      <c r="L1058" s="31"/>
+      <c r="M1058" s="29"/>
+      <c r="N1058" s="33"/>
+      <c r="P1058" s="29"/>
+      <c r="Q1058" s="32"/>
+      <c r="R1058" s="27"/>
+    </row>
+    <row r="1059" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1059" s="27"/>
+      <c r="B1059" s="39"/>
+      <c r="D1059" s="31"/>
+      <c r="E1059" s="33"/>
+      <c r="G1059" s="29"/>
+      <c r="H1059" s="31"/>
+      <c r="I1059" s="33"/>
+      <c r="K1059" s="29"/>
+      <c r="L1059" s="31"/>
+      <c r="M1059" s="29"/>
+      <c r="N1059" s="33"/>
+      <c r="P1059" s="29"/>
+      <c r="Q1059" s="32"/>
+      <c r="R1059" s="27"/>
+    </row>
+    <row r="1060" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1060" s="27"/>
+      <c r="B1060" s="39"/>
+      <c r="D1060" s="31"/>
+      <c r="E1060" s="33"/>
+      <c r="G1060" s="29"/>
+      <c r="H1060" s="31"/>
+      <c r="I1060" s="33"/>
+      <c r="K1060" s="29"/>
+      <c r="L1060" s="31"/>
+      <c r="M1060" s="29"/>
+      <c r="N1060" s="33"/>
+      <c r="P1060" s="29"/>
+      <c r="Q1060" s="32"/>
+      <c r="R1060" s="27"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" gridLines="1"/>
@@ -38713,9 +39172,9 @@
   </sheetPr>
   <dimension ref="A1:AB1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C15" sqref="C15"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -58285,7 +58744,7 @@
   </sheetPr>
   <dimension ref="A1:AB1030"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added new terms for brain
</commit_message>
<xml_diff>
--- a/flatmap_annotation.xlsx
+++ b/flatmap_annotation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Body organs" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="1129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="1141">
   <si>
     <t>Power point identifier</t>
   </si>
@@ -3411,13 +3411,49 @@
   </si>
   <si>
     <t xml:space="preserve">ILX:0727523 </t>
+  </si>
+  <si>
+    <t>brain_36</t>
+  </si>
+  <si>
+    <t>brain_37</t>
+  </si>
+  <si>
+    <t>brain_38</t>
+  </si>
+  <si>
+    <t>preoptic area</t>
+  </si>
+  <si>
+    <t>optic tract</t>
+  </si>
+  <si>
+    <t>basal forebrain</t>
+  </si>
+  <si>
+    <t>UBERON:0002743</t>
+  </si>
+  <si>
+    <t>ILX:0109225</t>
+  </si>
+  <si>
+    <t>ILX:0108074</t>
+  </si>
+  <si>
+    <t>UBERON:0001928</t>
+  </si>
+  <si>
+    <t>UBERON:0001908</t>
+  </si>
+  <si>
+    <t>ILX:0101101</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3473,6 +3509,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -3717,7 +3759,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3830,6 +3872,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4050,7 +4099,7 @@
   </sheetPr>
   <dimension ref="A1:AB1060"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+    <sheetView topLeftCell="A97" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
       <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
@@ -39169,9 +39218,9 @@
   </sheetPr>
   <dimension ref="A1:AB1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A6" sqref="A6:XFD6"/>
+      <selection pane="topRight" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -40433,15 +40482,26 @@
       <c r="Q38" s="27"/>
     </row>
     <row r="39" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A39" s="19"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="27"/>
+      <c r="A39" s="35" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B39" s="72" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D39" s="72" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E39" s="72" t="s">
+        <v>1138</v>
+      </c>
       <c r="F39" s="25"/>
       <c r="G39" s="27"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="27"/>
+      <c r="H39" s="72" t="s">
+        <v>1132</v>
+      </c>
+      <c r="I39" s="27" t="s">
+        <v>1136</v>
+      </c>
       <c r="J39" s="25"/>
       <c r="K39" s="27"/>
       <c r="L39" s="25"/>
@@ -40452,15 +40512,27 @@
       <c r="Q39" s="27"/>
     </row>
     <row r="40" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A40" s="19"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="27"/>
+      <c r="A40" s="45" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B40" s="72" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C40" s="62"/>
+      <c r="D40" s="74" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E40" s="72" t="s">
+        <v>1139</v>
+      </c>
       <c r="F40" s="25"/>
       <c r="G40" s="27"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="27"/>
+      <c r="H40" s="72" t="s">
+        <v>1133</v>
+      </c>
+      <c r="I40" s="27" t="s">
+        <v>1137</v>
+      </c>
       <c r="J40" s="25"/>
       <c r="K40" s="27"/>
       <c r="L40" s="25"/>
@@ -40471,15 +40543,27 @@
       <c r="Q40" s="27"/>
     </row>
     <row r="41" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A41" s="19"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="27"/>
+      <c r="A41" s="35" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B41" s="72" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C41" s="62"/>
+      <c r="D41" s="73" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E41" s="72" t="s">
+        <v>1135</v>
+      </c>
       <c r="F41" s="25"/>
       <c r="G41" s="27"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="27"/>
+      <c r="H41" s="73" t="s">
+        <v>1134</v>
+      </c>
+      <c r="I41" s="27" t="s">
+        <v>1140</v>
+      </c>
       <c r="J41" s="25"/>
       <c r="K41" s="27"/>
       <c r="L41" s="25"/>
@@ -40492,7 +40576,7 @@
     <row r="42" spans="1:17" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A42" s="19"/>
       <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
+      <c r="C42" s="32"/>
       <c r="D42" s="25"/>
       <c r="E42" s="27"/>
       <c r="F42" s="25"/>
@@ -58731,6 +58815,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added more annotation to brain
</commit_message>
<xml_diff>
--- a/flatmap_annotation.xlsx
+++ b/flatmap_annotation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Body organs" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="1165">
   <si>
     <t>Power point identifier</t>
   </si>
@@ -3447,6 +3447,78 @@
   </si>
   <si>
     <t>ILX:0101101</t>
+  </si>
+  <si>
+    <t>digestive_31</t>
+  </si>
+  <si>
+    <t>adrenal gland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0002369 </t>
+  </si>
+  <si>
+    <t>ILX:0731304</t>
+  </si>
+  <si>
+    <t>endocrine_3</t>
+  </si>
+  <si>
+    <t>UBERON:0002110</t>
+  </si>
+  <si>
+    <t>gall bladder</t>
+  </si>
+  <si>
+    <t>ILX:0727534</t>
+  </si>
+  <si>
+    <t>digestive_32</t>
+  </si>
+  <si>
+    <t>sigmoid colon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0001159 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILX:0729548 </t>
+  </si>
+  <si>
+    <t>reproductive_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0003889 </t>
+  </si>
+  <si>
+    <t>fallopian tube</t>
+  </si>
+  <si>
+    <t>ILX:0724851</t>
+  </si>
+  <si>
+    <t>submandibular gland</t>
+  </si>
+  <si>
+    <t>digestive_33</t>
+  </si>
+  <si>
+    <t>BERON:0001736</t>
+  </si>
+  <si>
+    <t>ILX:0724227</t>
+  </si>
+  <si>
+    <t>posterior vena cava</t>
+  </si>
+  <si>
+    <t>cardio_26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UBERON:0001072 </t>
+  </si>
+  <si>
+    <t>ILX:0736019</t>
   </si>
 </sst>
 </file>
@@ -4097,10 +4169,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB1060"/>
+  <dimension ref="A1:AB1066"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5137,7 +5209,7 @@
       <c r="C33" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="23" t="s">
+      <c r="D33" s="67" t="s">
         <v>529</v>
       </c>
       <c r="E33" s="26" t="s">
@@ -5842,14 +5914,26 @@
       <c r="R56" s="40"/>
     </row>
     <row r="57" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A57" s="19"/>
-      <c r="B57" s="39"/>
+      <c r="A57" s="35" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B57" s="35" t="s">
+        <v>1163</v>
+      </c>
       <c r="C57" s="21"/>
-      <c r="D57" s="23"/>
-      <c r="E57" s="26"/>
+      <c r="D57" s="67" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E57" s="43" t="s">
+        <v>1163</v>
+      </c>
       <c r="G57" s="29"/>
-      <c r="H57" s="23"/>
-      <c r="I57" s="26"/>
+      <c r="H57" s="42" t="s">
+        <v>1161</v>
+      </c>
+      <c r="I57" s="68" t="s">
+        <v>1164</v>
+      </c>
       <c r="K57" s="29"/>
       <c r="L57" s="31"/>
       <c r="M57" s="29"/>
@@ -5859,60 +5943,44 @@
       <c r="R57" s="40"/>
     </row>
     <row r="58" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A58" s="19" t="s">
-        <v>711</v>
-      </c>
-      <c r="B58" s="43" t="s">
-        <v>713</v>
-      </c>
-      <c r="C58" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D58" s="23" t="s">
-        <v>712</v>
-      </c>
-      <c r="E58" s="26" t="s">
-        <v>713</v>
-      </c>
+      <c r="A58" s="19"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="26"/>
       <c r="G58" s="29"/>
-      <c r="H58" s="23" t="s">
-        <v>712</v>
-      </c>
-      <c r="I58" s="26" t="s">
-        <v>714</v>
-      </c>
+      <c r="H58" s="23"/>
+      <c r="I58" s="26"/>
       <c r="K58" s="29"/>
       <c r="L58" s="31"/>
       <c r="M58" s="29"/>
       <c r="N58" s="33"/>
       <c r="P58" s="29"/>
       <c r="Q58" s="32"/>
-      <c r="R58" s="34" t="s">
-        <v>95</v>
-      </c>
+      <c r="R58" s="40"/>
     </row>
     <row r="59" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A59" s="19" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="B59" s="43" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="C59" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D59" s="23" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="E59" s="26" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="G59" s="29"/>
       <c r="H59" s="23" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="I59" s="26" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="K59" s="29"/>
       <c r="L59" s="31"/>
@@ -5920,32 +5988,32 @@
       <c r="N59" s="33"/>
       <c r="P59" s="29"/>
       <c r="Q59" s="32"/>
-      <c r="R59" s="34" t="b">
-        <v>1</v>
+      <c r="R59" s="34" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A60" s="19" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="B60" s="43" t="s">
-        <v>721</v>
-      </c>
-      <c r="C60" s="49" t="s">
-        <v>720</v>
+        <v>717</v>
+      </c>
+      <c r="C60" s="21" t="s">
+        <v>20</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="E60" s="26" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="G60" s="29"/>
       <c r="H60" s="23" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="I60" s="26" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="K60" s="29"/>
       <c r="L60" s="31"/>
@@ -5958,27 +6026,27 @@
       </c>
     </row>
     <row r="61" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A61" s="44" t="s">
-        <v>723</v>
+      <c r="A61" s="19" t="s">
+        <v>719</v>
       </c>
       <c r="B61" s="43" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="C61" s="49" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="D61" s="23" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="E61" s="26" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="G61" s="29"/>
       <c r="H61" s="23" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="I61" s="26" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="K61" s="29"/>
       <c r="L61" s="31"/>
@@ -5986,32 +6054,32 @@
       <c r="N61" s="33"/>
       <c r="P61" s="29"/>
       <c r="Q61" s="32"/>
-      <c r="R61" s="34" t="s">
-        <v>33</v>
+      <c r="R61" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A62" s="19" t="s">
-        <v>727</v>
+      <c r="A62" s="44" t="s">
+        <v>723</v>
       </c>
       <c r="B62" s="43" t="s">
-        <v>730</v>
-      </c>
-      <c r="C62" s="19" t="s">
-        <v>728</v>
-      </c>
-      <c r="D62" s="50" t="s">
-        <v>20</v>
+        <v>725</v>
+      </c>
+      <c r="C62" s="49" t="s">
+        <v>724</v>
+      </c>
+      <c r="D62" s="23" t="s">
+        <v>724</v>
       </c>
       <c r="E62" s="26" t="s">
-        <v>20</v>
+        <v>725</v>
       </c>
       <c r="G62" s="29"/>
       <c r="H62" s="23" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="I62" s="26" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="K62" s="29"/>
       <c r="L62" s="31"/>
@@ -6019,32 +6087,32 @@
       <c r="N62" s="33"/>
       <c r="P62" s="29"/>
       <c r="Q62" s="32"/>
-      <c r="R62" s="34" t="b">
-        <v>1</v>
+      <c r="R62" s="34" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A63" s="19" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="B63" s="43" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="C63" s="19" t="s">
+        <v>728</v>
+      </c>
+      <c r="D63" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D63" s="21" t="s">
-        <v>732</v>
-      </c>
       <c r="E63" s="26" t="s">
-        <v>733</v>
+        <v>20</v>
       </c>
       <c r="G63" s="29"/>
       <c r="H63" s="23" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="I63" s="26" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="K63" s="29"/>
       <c r="L63" s="31"/>
@@ -6052,32 +6120,32 @@
       <c r="N63" s="33"/>
       <c r="P63" s="29"/>
       <c r="Q63" s="32"/>
-      <c r="R63" s="34" t="s">
-        <v>33</v>
+      <c r="R63" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A64" s="44" t="s">
-        <v>735</v>
+      <c r="A64" s="19" t="s">
+        <v>731</v>
       </c>
       <c r="B64" s="43" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="C64" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D64" s="21" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="E64" s="26" t="s">
-        <v>20</v>
+        <v>733</v>
       </c>
       <c r="G64" s="29"/>
       <c r="H64" s="23" t="s">
-        <v>20</v>
+        <v>732</v>
       </c>
       <c r="I64" s="26" t="s">
-        <v>20</v>
+        <v>734</v>
       </c>
       <c r="K64" s="29"/>
       <c r="L64" s="31"/>
@@ -6090,21 +6158,27 @@
       </c>
     </row>
     <row r="65" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A65" s="44"/>
-      <c r="B65" s="39"/>
-      <c r="C65" s="19"/>
+      <c r="A65" s="44" t="s">
+        <v>735</v>
+      </c>
+      <c r="B65" s="43" t="s">
+        <v>738</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>20</v>
+      </c>
       <c r="D65" s="21" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E65" s="26" t="s">
-        <v>738</v>
+        <v>20</v>
       </c>
       <c r="G65" s="29"/>
       <c r="H65" s="23" t="s">
-        <v>737</v>
+        <v>20</v>
       </c>
       <c r="I65" s="26" t="s">
-        <v>739</v>
+        <v>20</v>
       </c>
       <c r="K65" s="29"/>
       <c r="L65" s="31"/>
@@ -6112,32 +6186,26 @@
       <c r="N65" s="33"/>
       <c r="P65" s="29"/>
       <c r="Q65" s="32"/>
-      <c r="R65" s="34" t="b">
-        <v>0</v>
+      <c r="R65" s="34" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A66" s="19" t="s">
-        <v>740</v>
-      </c>
-      <c r="B66" s="43" t="s">
-        <v>743</v>
-      </c>
-      <c r="C66" s="19" t="s">
-        <v>741</v>
-      </c>
+      <c r="A66" s="44"/>
+      <c r="B66" s="39"/>
+      <c r="C66" s="19"/>
       <c r="D66" s="21" t="s">
-        <v>20</v>
+        <v>737</v>
       </c>
       <c r="E66" s="26" t="s">
-        <v>20</v>
+        <v>738</v>
       </c>
       <c r="G66" s="29"/>
       <c r="H66" s="23" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="I66" s="26" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="K66" s="29"/>
       <c r="L66" s="31"/>
@@ -6145,32 +6213,32 @@
       <c r="N66" s="33"/>
       <c r="P66" s="29"/>
       <c r="Q66" s="32"/>
-      <c r="R66" s="34" t="s">
-        <v>33</v>
+      <c r="R66" s="34" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A67" s="19" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="B67" s="43" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="C67" s="19" t="s">
+        <v>741</v>
+      </c>
+      <c r="D67" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="21" t="s">
-        <v>745</v>
-      </c>
       <c r="E67" s="26" t="s">
-        <v>746</v>
+        <v>20</v>
       </c>
       <c r="G67" s="29"/>
       <c r="H67" s="23" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="I67" s="26" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="K67" s="29"/>
       <c r="L67" s="31"/>
@@ -6178,32 +6246,32 @@
       <c r="N67" s="33"/>
       <c r="P67" s="29"/>
       <c r="Q67" s="32"/>
-      <c r="R67" s="34" t="b">
-        <v>1</v>
+      <c r="R67" s="34" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A68" s="44" t="s">
-        <v>748</v>
+      <c r="A68" s="19" t="s">
+        <v>744</v>
       </c>
       <c r="B68" s="43" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="C68" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="E68" s="26" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="G68" s="29"/>
       <c r="H68" s="23" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="I68" s="26" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="K68" s="29"/>
       <c r="L68" s="31"/>
@@ -6216,27 +6284,27 @@
       </c>
     </row>
     <row r="69" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A69" s="19" t="s">
-        <v>752</v>
+      <c r="A69" s="44" t="s">
+        <v>748</v>
       </c>
       <c r="B69" s="43" t="s">
-        <v>755</v>
-      </c>
-      <c r="C69" s="21" t="s">
-        <v>753</v>
-      </c>
-      <c r="D69" s="23" t="s">
-        <v>754</v>
+        <v>750</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D69" s="21" t="s">
+        <v>749</v>
       </c>
       <c r="E69" s="26" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="G69" s="29"/>
       <c r="H69" s="23" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
       <c r="I69" s="26" t="s">
-        <v>756</v>
+        <v>751</v>
       </c>
       <c r="K69" s="29"/>
       <c r="L69" s="31"/>
@@ -6249,27 +6317,27 @@
       </c>
     </row>
     <row r="70" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A70" s="44" t="s">
-        <v>757</v>
+      <c r="A70" s="19" t="s">
+        <v>752</v>
       </c>
       <c r="B70" s="43" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>758</v>
+        <v>753</v>
       </c>
       <c r="D70" s="23" t="s">
-        <v>20</v>
+        <v>754</v>
       </c>
       <c r="E70" s="26" t="s">
-        <v>20</v>
+        <v>755</v>
       </c>
       <c r="G70" s="29"/>
       <c r="H70" s="23" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="I70" s="26" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="K70" s="29"/>
       <c r="L70" s="31"/>
@@ -6277,28 +6345,32 @@
       <c r="N70" s="33"/>
       <c r="P70" s="29"/>
       <c r="Q70" s="32"/>
-      <c r="R70" s="40"/>
+      <c r="R70" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="71" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A71" s="44" t="s">
-        <v>1074</v>
+        <v>757</v>
       </c>
       <c r="B71" s="43" t="s">
-        <v>1104</v>
-      </c>
-      <c r="C71" s="21"/>
-      <c r="D71" s="67" t="s">
-        <v>1103</v>
-      </c>
-      <c r="E71" s="43" t="s">
-        <v>1104</v>
+        <v>759</v>
+      </c>
+      <c r="C71" s="21" t="s">
+        <v>758</v>
+      </c>
+      <c r="D71" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E71" s="26" t="s">
+        <v>20</v>
       </c>
       <c r="G71" s="29"/>
-      <c r="H71" s="67" t="s">
-        <v>1103</v>
-      </c>
-      <c r="I71" s="68" t="s">
-        <v>1106</v>
+      <c r="H71" s="23" t="s">
+        <v>758</v>
+      </c>
+      <c r="I71" s="26" t="s">
+        <v>759</v>
       </c>
       <c r="K71" s="29"/>
       <c r="L71" s="31"/>
@@ -6309,25 +6381,25 @@
       <c r="R71" s="40"/>
     </row>
     <row r="72" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A72" s="35" t="s">
-        <v>1076</v>
+      <c r="A72" s="44" t="s">
+        <v>1074</v>
       </c>
       <c r="B72" s="43" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C72" s="21"/>
       <c r="D72" s="67" t="s">
-        <v>1075</v>
+        <v>1103</v>
       </c>
       <c r="E72" s="43" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="G72" s="29"/>
       <c r="H72" s="67" t="s">
-        <v>1075</v>
+        <v>1103</v>
       </c>
       <c r="I72" s="68" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="K72" s="29"/>
       <c r="L72" s="31"/>
@@ -6338,14 +6410,26 @@
       <c r="R72" s="40"/>
     </row>
     <row r="73" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A73" s="19"/>
-      <c r="B73" s="39"/>
+      <c r="A73" s="35" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B73" s="43" t="s">
+        <v>1105</v>
+      </c>
       <c r="C73" s="21"/>
-      <c r="D73" s="23"/>
-      <c r="E73" s="26"/>
+      <c r="D73" s="67" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E73" s="43" t="s">
+        <v>1105</v>
+      </c>
       <c r="G73" s="29"/>
-      <c r="H73" s="23"/>
-      <c r="I73" s="26"/>
+      <c r="H73" s="67" t="s">
+        <v>1075</v>
+      </c>
+      <c r="I73" s="68" t="s">
+        <v>1107</v>
+      </c>
       <c r="K73" s="29"/>
       <c r="L73" s="31"/>
       <c r="M73" s="29"/>
@@ -6355,60 +6439,44 @@
       <c r="R73" s="40"/>
     </row>
     <row r="74" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A74" s="19" t="s">
-        <v>760</v>
-      </c>
-      <c r="B74" s="43" t="s">
-        <v>762</v>
-      </c>
-      <c r="C74" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D74" s="23" t="s">
-        <v>761</v>
-      </c>
-      <c r="E74" s="26" t="s">
-        <v>762</v>
-      </c>
+      <c r="A74" s="19"/>
+      <c r="B74" s="39"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="26"/>
       <c r="G74" s="29"/>
-      <c r="H74" s="42" t="s">
-        <v>761</v>
-      </c>
-      <c r="I74" s="26" t="s">
-        <v>763</v>
-      </c>
+      <c r="H74" s="23"/>
+      <c r="I74" s="26"/>
       <c r="K74" s="29"/>
       <c r="L74" s="31"/>
       <c r="M74" s="29"/>
       <c r="N74" s="33"/>
       <c r="P74" s="29"/>
       <c r="Q74" s="32"/>
-      <c r="R74" s="34" t="s">
-        <v>764</v>
-      </c>
+      <c r="R74" s="40"/>
     </row>
     <row r="75" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A75" s="19" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="B75" s="43" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="C75" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D75" s="23" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E75" s="26" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="G75" s="29"/>
-      <c r="H75" s="23" t="s">
-        <v>766</v>
+      <c r="H75" s="42" t="s">
+        <v>761</v>
       </c>
       <c r="I75" s="26" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
       <c r="K75" s="29"/>
       <c r="L75" s="31"/>
@@ -6416,32 +6484,32 @@
       <c r="N75" s="33"/>
       <c r="P75" s="29"/>
       <c r="Q75" s="32"/>
-      <c r="R75" s="34" t="b">
-        <v>1</v>
+      <c r="R75" s="34" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="76" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A76" s="19" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="B76" s="43" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="C76" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D76" s="42" t="s">
-        <v>770</v>
+      <c r="D76" s="23" t="s">
+        <v>766</v>
       </c>
       <c r="E76" s="26" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="G76" s="29"/>
-      <c r="H76" s="42" t="s">
-        <v>770</v>
+      <c r="H76" s="23" t="s">
+        <v>766</v>
       </c>
       <c r="I76" s="26" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="K76" s="29"/>
       <c r="L76" s="31"/>
@@ -6455,26 +6523,26 @@
     </row>
     <row r="77" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A77" s="19" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="B77" s="43" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="C77" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D77" s="42" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="E77" s="26" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="G77" s="29"/>
       <c r="H77" s="42" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="I77" s="26" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="K77" s="29"/>
       <c r="L77" s="31"/>
@@ -6482,32 +6550,32 @@
       <c r="N77" s="33"/>
       <c r="P77" s="29"/>
       <c r="Q77" s="32"/>
-      <c r="R77" s="34" t="s">
-        <v>95</v>
+      <c r="R77" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A78" s="19" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="B78" s="43" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="C78" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D78" s="23" t="s">
-        <v>778</v>
+      <c r="D78" s="42" t="s">
+        <v>774</v>
       </c>
       <c r="E78" s="26" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="G78" s="29"/>
-      <c r="H78" s="23" t="s">
-        <v>778</v>
+      <c r="H78" s="42" t="s">
+        <v>774</v>
       </c>
       <c r="I78" s="26" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="K78" s="29"/>
       <c r="L78" s="31"/>
@@ -6516,31 +6584,31 @@
       <c r="P78" s="29"/>
       <c r="Q78" s="32"/>
       <c r="R78" s="34" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
     </row>
     <row r="79" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A79" s="19" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="B79" s="43" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="C79" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D79" s="23" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="E79" s="26" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="G79" s="29"/>
       <c r="H79" s="23" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="I79" s="26" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="K79" s="29"/>
       <c r="L79" s="31"/>
@@ -6548,32 +6616,32 @@
       <c r="N79" s="33"/>
       <c r="P79" s="29"/>
       <c r="Q79" s="32"/>
-      <c r="R79" s="34" t="b">
-        <v>1</v>
+      <c r="R79" s="34" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="80" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A80" s="19" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="B80" s="43" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="C80" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D80" s="23" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="E80" s="26" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="G80" s="29"/>
       <c r="H80" s="23" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="I80" s="26" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="K80" s="29"/>
       <c r="L80" s="31"/>
@@ -6587,26 +6655,26 @@
     </row>
     <row r="81" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A81" s="19" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="B81" s="43" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C81" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D81" s="23" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="E81" s="26" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="G81" s="29"/>
       <c r="H81" s="23" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="I81" s="26" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="K81" s="29"/>
       <c r="L81" s="31"/>
@@ -6614,32 +6682,32 @@
       <c r="N81" s="33"/>
       <c r="P81" s="29"/>
       <c r="Q81" s="32"/>
-      <c r="R81" s="34" t="s">
-        <v>33</v>
+      <c r="R81" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A82" s="19" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="B82" s="43" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="C82" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D82" s="23" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="E82" s="26" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="G82" s="29"/>
       <c r="H82" s="23" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="I82" s="26" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="K82" s="29"/>
       <c r="L82" s="31"/>
@@ -6647,32 +6715,32 @@
       <c r="N82" s="33"/>
       <c r="P82" s="29"/>
       <c r="Q82" s="32"/>
-      <c r="R82" s="34" t="b">
-        <v>1</v>
+      <c r="R82" s="34" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="83" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A83" s="19" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="B83" s="43" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="C83" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D83" s="23" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="E83" s="26" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="G83" s="29"/>
       <c r="H83" s="23" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="I83" s="26" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="K83" s="29"/>
       <c r="L83" s="31"/>
@@ -6686,26 +6754,26 @@
     </row>
     <row r="84" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A84" s="19" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="B84" s="43" t="s">
-        <v>804</v>
-      </c>
-      <c r="C84" s="50" t="s">
-        <v>802</v>
+        <v>799</v>
+      </c>
+      <c r="C84" s="21" t="s">
+        <v>20</v>
       </c>
       <c r="D84" s="23" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
       <c r="E84" s="26" t="s">
-        <v>804</v>
+        <v>799</v>
       </c>
       <c r="G84" s="29"/>
       <c r="H84" s="23" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
       <c r="I84" s="26" t="s">
-        <v>805</v>
+        <v>800</v>
       </c>
       <c r="K84" s="29"/>
       <c r="L84" s="31"/>
@@ -6719,26 +6787,26 @@
     </row>
     <row r="85" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A85" s="19" t="s">
-        <v>806</v>
+        <v>801</v>
       </c>
       <c r="B85" s="43" t="s">
-        <v>809</v>
+        <v>804</v>
       </c>
       <c r="C85" s="50" t="s">
-        <v>807</v>
+        <v>802</v>
       </c>
       <c r="D85" s="23" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
       <c r="E85" s="26" t="s">
-        <v>809</v>
+        <v>804</v>
       </c>
       <c r="G85" s="29"/>
       <c r="H85" s="23" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
       <c r="I85" s="26" t="s">
-        <v>810</v>
+        <v>805</v>
       </c>
       <c r="K85" s="29"/>
       <c r="L85" s="31"/>
@@ -6752,26 +6820,26 @@
     </row>
     <row r="86" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A86" s="19" t="s">
-        <v>811</v>
+        <v>806</v>
       </c>
       <c r="B86" s="43" t="s">
-        <v>813</v>
-      </c>
-      <c r="C86" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D86" s="21" t="s">
-        <v>812</v>
+        <v>809</v>
+      </c>
+      <c r="C86" s="50" t="s">
+        <v>807</v>
+      </c>
+      <c r="D86" s="23" t="s">
+        <v>808</v>
       </c>
       <c r="E86" s="26" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="G86" s="29"/>
       <c r="H86" s="23" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="I86" s="26" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="K86" s="29"/>
       <c r="L86" s="31"/>
@@ -6785,26 +6853,26 @@
     </row>
     <row r="87" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A87" s="19" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="B87" s="43" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="C87" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D87" s="21" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="E87" s="26" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="G87" s="29"/>
       <c r="H87" s="23" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="I87" s="26" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="K87" s="29"/>
       <c r="L87" s="31"/>
@@ -6818,26 +6886,26 @@
     </row>
     <row r="88" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A88" s="19" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="B88" s="43" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="C88" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D88" s="21" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="E88" s="26" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="G88" s="29"/>
       <c r="H88" s="23" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="I88" s="26" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="K88" s="29"/>
       <c r="L88" s="31"/>
@@ -6851,26 +6919,26 @@
     </row>
     <row r="89" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A89" s="19" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="B89" s="43" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="C89" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D89" s="21" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="E89" s="26" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="G89" s="29"/>
       <c r="H89" s="23" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="I89" s="26" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="K89" s="29"/>
       <c r="L89" s="31"/>
@@ -6878,32 +6946,32 @@
       <c r="N89" s="33"/>
       <c r="P89" s="29"/>
       <c r="Q89" s="32"/>
-      <c r="R89" s="34" t="s">
-        <v>827</v>
+      <c r="R89" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A90" s="19" t="s">
-        <v>828</v>
+        <v>823</v>
       </c>
       <c r="B90" s="43" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="C90" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>829</v>
+        <v>824</v>
       </c>
       <c r="E90" s="26" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="G90" s="29"/>
       <c r="H90" s="23" t="s">
-        <v>829</v>
+        <v>824</v>
       </c>
       <c r="I90" s="26" t="s">
-        <v>831</v>
+        <v>826</v>
       </c>
       <c r="K90" s="29"/>
       <c r="L90" s="31"/>
@@ -6912,31 +6980,31 @@
       <c r="P90" s="29"/>
       <c r="Q90" s="32"/>
       <c r="R90" s="34" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
     </row>
     <row r="91" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A91" s="65" t="s">
-        <v>1060</v>
+      <c r="A91" s="19" t="s">
+        <v>828</v>
       </c>
       <c r="B91" s="43" t="s">
-        <v>1078</v>
-      </c>
-      <c r="C91" s="59" t="s">
+        <v>830</v>
+      </c>
+      <c r="C91" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D91" s="21" t="s">
-        <v>1077</v>
-      </c>
-      <c r="E91" s="43" t="s">
-        <v>1078</v>
+        <v>829</v>
+      </c>
+      <c r="E91" s="26" t="s">
+        <v>830</v>
       </c>
       <c r="G91" s="29"/>
-      <c r="H91" s="21" t="s">
-        <v>1077</v>
-      </c>
-      <c r="I91" s="43" t="s">
-        <v>1079</v>
+      <c r="H91" s="23" t="s">
+        <v>829</v>
+      </c>
+      <c r="I91" s="26" t="s">
+        <v>831</v>
       </c>
       <c r="K91" s="29"/>
       <c r="L91" s="31"/>
@@ -6944,30 +7012,32 @@
       <c r="N91" s="33"/>
       <c r="P91" s="29"/>
       <c r="Q91" s="32"/>
-      <c r="R91" s="40"/>
+      <c r="R91" s="34" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="92" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A92" s="35" t="s">
-        <v>1061</v>
+      <c r="A92" s="65" t="s">
+        <v>1060</v>
       </c>
       <c r="B92" s="43" t="s">
-        <v>1064</v>
+        <v>1078</v>
       </c>
       <c r="C92" s="59" t="s">
         <v>20</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>1063</v>
+        <v>1077</v>
       </c>
       <c r="E92" s="43" t="s">
-        <v>1064</v>
+        <v>1078</v>
       </c>
       <c r="G92" s="29"/>
       <c r="H92" s="21" t="s">
-        <v>1063</v>
+        <v>1077</v>
       </c>
       <c r="I92" s="43" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="K92" s="29"/>
       <c r="L92" s="31"/>
@@ -6979,26 +7049,26 @@
     </row>
     <row r="93" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A93" s="35" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B93" s="43" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="C93" s="59" t="s">
         <v>20</v>
       </c>
       <c r="D93" s="21" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="E93" s="43" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="G93" s="29"/>
       <c r="H93" s="21" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="I93" s="43" t="s">
-        <v>1066</v>
+        <v>1080</v>
       </c>
       <c r="K93" s="29"/>
       <c r="L93" s="31"/>
@@ -7010,26 +7080,26 @@
     </row>
     <row r="94" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A94" s="35" t="s">
-        <v>1068</v>
+        <v>1062</v>
       </c>
       <c r="B94" s="43" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="C94" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="D94" s="66" t="s">
-        <v>1071</v>
+      <c r="D94" s="21" t="s">
+        <v>1065</v>
       </c>
       <c r="E94" s="43" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="G94" s="29"/>
-      <c r="H94" s="66" t="s">
-        <v>1071</v>
+      <c r="H94" s="21" t="s">
+        <v>1065</v>
       </c>
       <c r="I94" s="43" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="K94" s="29"/>
       <c r="L94" s="31"/>
@@ -7041,17 +7111,27 @@
     </row>
     <row r="95" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A95" s="35" t="s">
-        <v>1081</v>
-      </c>
-      <c r="B95" s="35"/>
-      <c r="C95" s="59"/>
+        <v>1068</v>
+      </c>
+      <c r="B95" s="43" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C95" s="59" t="s">
+        <v>20</v>
+      </c>
       <c r="D95" s="66" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E95" s="43"/>
+        <v>1071</v>
+      </c>
+      <c r="E95" s="43" t="s">
+        <v>1070</v>
+      </c>
       <c r="G95" s="29"/>
-      <c r="H95" s="66"/>
-      <c r="I95" s="43"/>
+      <c r="H95" s="66" t="s">
+        <v>1071</v>
+      </c>
+      <c r="I95" s="43" t="s">
+        <v>1069</v>
+      </c>
       <c r="K95" s="29"/>
       <c r="L95" s="31"/>
       <c r="M95" s="29"/>
@@ -7062,12 +7142,12 @@
     </row>
     <row r="96" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A96" s="35" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B96" s="35"/>
       <c r="C96" s="59"/>
       <c r="D96" s="66" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="E96" s="43"/>
       <c r="G96" s="29"/>
@@ -7083,25 +7163,17 @@
     </row>
     <row r="97" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A97" s="35" t="s">
-        <v>1085</v>
-      </c>
-      <c r="B97" s="43" t="s">
-        <v>1088</v>
-      </c>
+        <v>1082</v>
+      </c>
+      <c r="B97" s="35"/>
       <c r="C97" s="59"/>
       <c r="D97" s="66" t="s">
-        <v>1087</v>
-      </c>
-      <c r="E97" s="43" t="s">
-        <v>1088</v>
-      </c>
+        <v>1084</v>
+      </c>
+      <c r="E97" s="43"/>
       <c r="G97" s="29"/>
-      <c r="H97" s="66" t="s">
-        <v>1087</v>
-      </c>
-      <c r="I97" s="43" t="s">
-        <v>1089</v>
-      </c>
+      <c r="H97" s="66"/>
+      <c r="I97" s="43"/>
       <c r="K97" s="29"/>
       <c r="L97" s="31"/>
       <c r="M97" s="29"/>
@@ -7112,24 +7184,24 @@
     </row>
     <row r="98" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A98" s="35" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B98" s="43" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
       <c r="C98" s="59"/>
-      <c r="D98" s="21" t="s">
-        <v>1091</v>
+      <c r="D98" s="66" t="s">
+        <v>1087</v>
       </c>
       <c r="E98" s="43" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
       <c r="G98" s="29"/>
-      <c r="H98" s="21" t="s">
-        <v>1091</v>
+      <c r="H98" s="66" t="s">
+        <v>1087</v>
       </c>
       <c r="I98" s="43" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="K98" s="29"/>
       <c r="L98" s="31"/>
@@ -7141,24 +7213,24 @@
     </row>
     <row r="99" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A99" s="35" t="s">
-        <v>1095</v>
+        <v>1086</v>
       </c>
       <c r="B99" s="43" t="s">
-        <v>1109</v>
+        <v>1092</v>
       </c>
       <c r="C99" s="59"/>
-      <c r="D99" s="66" t="s">
-        <v>1108</v>
+      <c r="D99" s="21" t="s">
+        <v>1091</v>
       </c>
       <c r="E99" s="43" t="s">
-        <v>1109</v>
+        <v>1092</v>
       </c>
       <c r="G99" s="29"/>
-      <c r="H99" s="66" t="s">
-        <v>1108</v>
-      </c>
-      <c r="I99" s="68" t="s">
-        <v>1110</v>
+      <c r="H99" s="21" t="s">
+        <v>1091</v>
+      </c>
+      <c r="I99" s="43" t="s">
+        <v>1090</v>
       </c>
       <c r="K99" s="29"/>
       <c r="L99" s="31"/>
@@ -7170,24 +7242,24 @@
     </row>
     <row r="100" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A100" s="35" t="s">
-        <v>1100</v>
+        <v>1095</v>
       </c>
       <c r="B100" s="43" t="s">
-        <v>1102</v>
+        <v>1109</v>
       </c>
       <c r="C100" s="59"/>
       <c r="D100" s="66" t="s">
-        <v>1101</v>
+        <v>1108</v>
       </c>
       <c r="E100" s="43" t="s">
-        <v>1102</v>
+        <v>1109</v>
       </c>
       <c r="G100" s="29"/>
       <c r="H100" s="66" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="I100" s="68" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="K100" s="29"/>
       <c r="L100" s="31"/>
@@ -7199,26 +7271,24 @@
     </row>
     <row r="101" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A101" s="35" t="s">
-        <v>1117</v>
-      </c>
-      <c r="B101" s="68" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C101" s="71" t="s">
-        <v>1119</v>
-      </c>
+        <v>1100</v>
+      </c>
+      <c r="B101" s="43" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C101" s="59"/>
       <c r="D101" s="66" t="s">
-        <v>1120</v>
-      </c>
-      <c r="E101" s="68" t="s">
-        <v>1121</v>
+        <v>1101</v>
+      </c>
+      <c r="E101" s="43" t="s">
+        <v>1102</v>
       </c>
       <c r="G101" s="29"/>
       <c r="H101" s="66" t="s">
-        <v>1120</v>
+        <v>1112</v>
       </c>
       <c r="I101" s="68" t="s">
-        <v>1122</v>
+        <v>1111</v>
       </c>
       <c r="K101" s="29"/>
       <c r="L101" s="31"/>
@@ -7230,24 +7300,26 @@
     </row>
     <row r="102" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A102" s="35" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B102" s="68" t="s">
-        <v>821</v>
-      </c>
-      <c r="C102" s="59"/>
+        <v>1121</v>
+      </c>
+      <c r="C102" s="71" t="s">
+        <v>1119</v>
+      </c>
       <c r="D102" s="66" t="s">
-        <v>820</v>
+        <v>1120</v>
       </c>
       <c r="E102" s="68" t="s">
-        <v>821</v>
+        <v>1121</v>
       </c>
       <c r="G102" s="29"/>
       <c r="H102" s="66" t="s">
-        <v>820</v>
+        <v>1120</v>
       </c>
       <c r="I102" s="68" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="K102" s="29"/>
       <c r="L102" s="31"/>
@@ -7259,26 +7331,24 @@
     </row>
     <row r="103" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A103" s="35" t="s">
-        <v>1123</v>
+        <v>1118</v>
       </c>
       <c r="B103" s="68" t="s">
-        <v>1127</v>
-      </c>
-      <c r="C103" s="71" t="s">
-        <v>1125</v>
-      </c>
+        <v>821</v>
+      </c>
+      <c r="C103" s="59"/>
       <c r="D103" s="66" t="s">
-        <v>1126</v>
+        <v>820</v>
       </c>
       <c r="E103" s="68" t="s">
-        <v>1127</v>
+        <v>821</v>
       </c>
       <c r="G103" s="29"/>
       <c r="H103" s="66" t="s">
-        <v>1126</v>
+        <v>820</v>
       </c>
       <c r="I103" s="68" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="K103" s="29"/>
       <c r="L103" s="31"/>
@@ -7289,13 +7359,28 @@
       <c r="R103" s="40"/>
     </row>
     <row r="104" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A104" s="27"/>
-      <c r="B104" s="39"/>
-      <c r="D104" s="31"/>
-      <c r="E104" s="33"/>
+      <c r="A104" s="35" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B104" s="68" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C104" s="71" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D104" s="66" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E104" s="68" t="s">
+        <v>1127</v>
+      </c>
       <c r="G104" s="29"/>
-      <c r="H104" s="31"/>
-      <c r="I104" s="33"/>
+      <c r="H104" s="66" t="s">
+        <v>1126</v>
+      </c>
+      <c r="I104" s="68" t="s">
+        <v>1128</v>
+      </c>
       <c r="K104" s="29"/>
       <c r="L104" s="31"/>
       <c r="M104" s="29"/>
@@ -7305,27 +7390,25 @@
       <c r="R104" s="40"/>
     </row>
     <row r="105" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A105" s="19" t="s">
-        <v>833</v>
-      </c>
-      <c r="B105" s="43" t="s">
-        <v>835</v>
-      </c>
-      <c r="C105" s="21" t="s">
-        <v>834</v>
-      </c>
-      <c r="D105" s="23" t="s">
-        <v>834</v>
-      </c>
-      <c r="E105" s="26" t="s">
-        <v>835</v>
+      <c r="A105" s="35" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B105" s="68" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C105" s="71"/>
+      <c r="D105" s="66" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E105" s="68" t="s">
+        <v>1146</v>
       </c>
       <c r="G105" s="29"/>
-      <c r="H105" s="23" t="s">
-        <v>834</v>
-      </c>
-      <c r="I105" s="26" t="s">
-        <v>836</v>
+      <c r="H105" s="66" t="s">
+        <v>1147</v>
+      </c>
+      <c r="I105" s="68" t="s">
+        <v>1148</v>
       </c>
       <c r="K105" s="29"/>
       <c r="L105" s="31"/>
@@ -7333,32 +7416,28 @@
       <c r="N105" s="33"/>
       <c r="P105" s="29"/>
       <c r="Q105" s="32"/>
-      <c r="R105" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R105" s="40"/>
     </row>
     <row r="106" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A106" s="19" t="s">
-        <v>837</v>
-      </c>
-      <c r="B106" s="43" t="s">
-        <v>839</v>
-      </c>
-      <c r="C106" s="21" t="s">
-        <v>838</v>
-      </c>
-      <c r="D106" s="23" t="s">
-        <v>838</v>
-      </c>
-      <c r="E106" s="26" t="s">
-        <v>839</v>
+      <c r="A106" s="35" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B106" s="65" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C106" s="71"/>
+      <c r="D106" s="66" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E106" s="68" t="s">
+        <v>1151</v>
       </c>
       <c r="G106" s="29"/>
-      <c r="H106" s="23" t="s">
-        <v>838</v>
-      </c>
-      <c r="I106" s="26" t="s">
-        <v>840</v>
+      <c r="H106" s="66" t="s">
+        <v>1150</v>
+      </c>
+      <c r="I106" s="68" t="s">
+        <v>1152</v>
       </c>
       <c r="K106" s="29"/>
       <c r="L106" s="31"/>
@@ -7366,32 +7445,28 @@
       <c r="N106" s="33"/>
       <c r="P106" s="29"/>
       <c r="Q106" s="32"/>
-      <c r="R106" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R106" s="40"/>
     </row>
     <row r="107" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A107" s="19" t="s">
-        <v>841</v>
-      </c>
-      <c r="B107" s="43" t="s">
-        <v>843</v>
-      </c>
-      <c r="C107" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D107" s="23" t="s">
-        <v>842</v>
-      </c>
-      <c r="E107" s="26" t="s">
-        <v>843</v>
+      <c r="A107" s="35" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B107" s="65" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C107" s="71"/>
+      <c r="D107" s="66" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E107" s="68" t="s">
+        <v>1159</v>
       </c>
       <c r="G107" s="29"/>
-      <c r="H107" s="42" t="s">
-        <v>842</v>
-      </c>
-      <c r="I107" s="26" t="s">
-        <v>844</v>
+      <c r="H107" s="66" t="s">
+        <v>1157</v>
+      </c>
+      <c r="I107" s="68" t="s">
+        <v>1160</v>
       </c>
       <c r="K107" s="29"/>
       <c r="L107" s="31"/>
@@ -7399,65 +7474,46 @@
       <c r="N107" s="33"/>
       <c r="P107" s="29"/>
       <c r="Q107" s="32"/>
-      <c r="R107" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R107" s="40"/>
     </row>
     <row r="108" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A108" s="19" t="s">
-        <v>845</v>
-      </c>
-      <c r="B108" s="43" t="s">
-        <v>847</v>
-      </c>
-      <c r="C108" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D108" s="23" t="s">
-        <v>846</v>
-      </c>
-      <c r="E108" s="26" t="s">
-        <v>847</v>
-      </c>
+      <c r="A108" s="27"/>
+      <c r="B108" s="39"/>
+      <c r="D108" s="31"/>
+      <c r="E108" s="33"/>
       <c r="G108" s="29"/>
-      <c r="H108" s="42" t="s">
-        <v>846</v>
-      </c>
-      <c r="I108" s="26" t="s">
-        <v>848</v>
-      </c>
+      <c r="H108" s="31"/>
+      <c r="I108" s="33"/>
       <c r="K108" s="29"/>
       <c r="L108" s="31"/>
       <c r="M108" s="29"/>
       <c r="N108" s="33"/>
       <c r="P108" s="29"/>
       <c r="Q108" s="32"/>
-      <c r="R108" s="34" t="s">
-        <v>849</v>
-      </c>
+      <c r="R108" s="40"/>
     </row>
     <row r="109" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A109" s="19" t="s">
-        <v>850</v>
+        <v>833</v>
       </c>
       <c r="B109" s="43" t="s">
-        <v>852</v>
+        <v>835</v>
       </c>
       <c r="C109" s="21" t="s">
-        <v>20</v>
+        <v>834</v>
       </c>
       <c r="D109" s="23" t="s">
-        <v>851</v>
+        <v>834</v>
       </c>
       <c r="E109" s="26" t="s">
-        <v>852</v>
+        <v>835</v>
       </c>
       <c r="G109" s="29"/>
-      <c r="H109" s="42" t="s">
-        <v>851</v>
+      <c r="H109" s="23" t="s">
+        <v>834</v>
       </c>
       <c r="I109" s="26" t="s">
-        <v>853</v>
+        <v>836</v>
       </c>
       <c r="K109" s="29"/>
       <c r="L109" s="31"/>
@@ -7470,25 +7526,27 @@
       </c>
     </row>
     <row r="110" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A110" s="35" t="s">
-        <v>1093</v>
-      </c>
-      <c r="B110" s="68" t="s">
-        <v>1113</v>
-      </c>
-      <c r="C110" s="21"/>
-      <c r="D110" s="67" t="s">
-        <v>1094</v>
-      </c>
-      <c r="E110" s="68" t="s">
-        <v>1113</v>
+      <c r="A110" s="65" t="s">
+        <v>837</v>
+      </c>
+      <c r="B110" s="43" t="s">
+        <v>839</v>
+      </c>
+      <c r="C110" s="21" t="s">
+        <v>838</v>
+      </c>
+      <c r="D110" s="23" t="s">
+        <v>838</v>
+      </c>
+      <c r="E110" s="26" t="s">
+        <v>839</v>
       </c>
       <c r="G110" s="29"/>
-      <c r="H110" s="67" t="s">
-        <v>1094</v>
-      </c>
-      <c r="I110" s="43" t="s">
-        <v>1114</v>
+      <c r="H110" s="23" t="s">
+        <v>838</v>
+      </c>
+      <c r="I110" s="26" t="s">
+        <v>840</v>
       </c>
       <c r="K110" s="29"/>
       <c r="L110" s="31"/>
@@ -7496,28 +7554,32 @@
       <c r="N110" s="33"/>
       <c r="P110" s="29"/>
       <c r="Q110" s="32"/>
-      <c r="R110" s="40"/>
+      <c r="R110" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="111" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A111" s="35" t="s">
-        <v>1096</v>
+      <c r="A111" s="19" t="s">
+        <v>841</v>
       </c>
       <c r="B111" s="43" t="s">
-        <v>1098</v>
-      </c>
-      <c r="C111" s="21"/>
-      <c r="D111" s="42" t="s">
-        <v>1097</v>
-      </c>
-      <c r="E111" s="43" t="s">
-        <v>1098</v>
+        <v>843</v>
+      </c>
+      <c r="C111" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D111" s="23" t="s">
+        <v>842</v>
+      </c>
+      <c r="E111" s="26" t="s">
+        <v>843</v>
       </c>
       <c r="G111" s="29"/>
       <c r="H111" s="42" t="s">
-        <v>1097</v>
-      </c>
-      <c r="I111" s="43" t="s">
-        <v>1099</v>
+        <v>842</v>
+      </c>
+      <c r="I111" s="26" t="s">
+        <v>844</v>
       </c>
       <c r="K111" s="29"/>
       <c r="L111" s="31"/>
@@ -7525,46 +7587,65 @@
       <c r="N111" s="33"/>
       <c r="P111" s="29"/>
       <c r="Q111" s="32"/>
-      <c r="R111" s="40"/>
+      <c r="R111" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="112" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A112" s="27"/>
-      <c r="B112" s="39"/>
-      <c r="D112" s="31"/>
-      <c r="E112" s="33"/>
+      <c r="A112" s="19" t="s">
+        <v>845</v>
+      </c>
+      <c r="B112" s="43" t="s">
+        <v>847</v>
+      </c>
+      <c r="C112" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D112" s="23" t="s">
+        <v>846</v>
+      </c>
+      <c r="E112" s="26" t="s">
+        <v>847</v>
+      </c>
       <c r="G112" s="29"/>
-      <c r="H112" s="31"/>
-      <c r="I112" s="33"/>
+      <c r="H112" s="42" t="s">
+        <v>846</v>
+      </c>
+      <c r="I112" s="26" t="s">
+        <v>848</v>
+      </c>
       <c r="K112" s="29"/>
       <c r="L112" s="31"/>
       <c r="M112" s="29"/>
       <c r="N112" s="33"/>
       <c r="P112" s="29"/>
       <c r="Q112" s="32"/>
-      <c r="R112" s="34"/>
+      <c r="R112" s="34" t="s">
+        <v>849</v>
+      </c>
     </row>
     <row r="113" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A113" s="19" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="B113" s="43" t="s">
-        <v>857</v>
+        <v>852</v>
       </c>
       <c r="C113" s="21" t="s">
-        <v>855</v>
+        <v>20</v>
       </c>
       <c r="D113" s="23" t="s">
-        <v>20</v>
+        <v>851</v>
       </c>
       <c r="E113" s="26" t="s">
-        <v>20</v>
+        <v>852</v>
       </c>
       <c r="G113" s="29"/>
-      <c r="H113" s="23" t="s">
-        <v>856</v>
+      <c r="H113" s="42" t="s">
+        <v>851</v>
       </c>
       <c r="I113" s="26" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="K113" s="29"/>
       <c r="L113" s="31"/>
@@ -7572,19 +7653,31 @@
       <c r="N113" s="33"/>
       <c r="P113" s="29"/>
       <c r="Q113" s="32"/>
-      <c r="R113" s="34" t="s">
-        <v>849</v>
+      <c r="R113" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A114" s="19"/>
-      <c r="B114" s="39"/>
+      <c r="A114" s="35" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B114" s="68" t="s">
+        <v>1113</v>
+      </c>
       <c r="C114" s="21"/>
-      <c r="D114" s="31"/>
-      <c r="E114" s="33"/>
+      <c r="D114" s="67" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E114" s="68" t="s">
+        <v>1113</v>
+      </c>
       <c r="G114" s="29"/>
-      <c r="H114" s="31"/>
-      <c r="I114" s="33"/>
+      <c r="H114" s="67" t="s">
+        <v>1094</v>
+      </c>
+      <c r="I114" s="43" t="s">
+        <v>1114</v>
+      </c>
       <c r="K114" s="29"/>
       <c r="L114" s="31"/>
       <c r="M114" s="29"/>
@@ -7594,27 +7687,25 @@
       <c r="R114" s="40"/>
     </row>
     <row r="115" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A115" s="19" t="s">
-        <v>858</v>
+      <c r="A115" s="35" t="s">
+        <v>1096</v>
       </c>
       <c r="B115" s="43" t="s">
-        <v>860</v>
-      </c>
-      <c r="C115" s="19" t="s">
-        <v>859</v>
-      </c>
-      <c r="D115" s="21" t="s">
-        <v>859</v>
-      </c>
-      <c r="E115" s="26" t="s">
-        <v>860</v>
-      </c>
-      <c r="G115" s="33"/>
-      <c r="H115" s="21" t="s">
-        <v>859</v>
-      </c>
-      <c r="I115" s="26" t="s">
-        <v>861</v>
+        <v>1098</v>
+      </c>
+      <c r="C115" s="21"/>
+      <c r="D115" s="42" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E115" s="43" t="s">
+        <v>1098</v>
+      </c>
+      <c r="G115" s="29"/>
+      <c r="H115" s="42" t="s">
+        <v>1097</v>
+      </c>
+      <c r="I115" s="43" t="s">
+        <v>1099</v>
       </c>
       <c r="K115" s="29"/>
       <c r="L115" s="31"/>
@@ -7622,32 +7713,28 @@
       <c r="N115" s="33"/>
       <c r="P115" s="29"/>
       <c r="Q115" s="32"/>
-      <c r="R115" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R115" s="40"/>
     </row>
     <row r="116" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A116" s="19" t="s">
-        <v>862</v>
-      </c>
-      <c r="B116" s="43" t="s">
-        <v>864</v>
-      </c>
-      <c r="C116" s="21" t="s">
-        <v>863</v>
-      </c>
-      <c r="D116" s="23" t="s">
-        <v>863</v>
-      </c>
-      <c r="E116" s="26" t="s">
-        <v>864</v>
+      <c r="A116" s="35" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B116" s="35" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C116" s="21"/>
+      <c r="D116" s="67" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E116" s="35" t="s">
+        <v>1154</v>
       </c>
       <c r="G116" s="29"/>
-      <c r="H116" s="23" t="s">
-        <v>863</v>
-      </c>
-      <c r="I116" s="26" t="s">
-        <v>865</v>
+      <c r="H116" s="42" t="s">
+        <v>1155</v>
+      </c>
+      <c r="I116" s="43" t="s">
+        <v>1156</v>
       </c>
       <c r="K116" s="29"/>
       <c r="L116" s="31"/>
@@ -7655,9 +7742,7 @@
       <c r="N116" s="33"/>
       <c r="P116" s="29"/>
       <c r="Q116" s="32"/>
-      <c r="R116" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R116" s="40"/>
     </row>
     <row r="117" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A117" s="27"/>
@@ -7673,30 +7758,30 @@
       <c r="N117" s="33"/>
       <c r="P117" s="29"/>
       <c r="Q117" s="32"/>
-      <c r="R117" s="40"/>
+      <c r="R117" s="34"/>
     </row>
     <row r="118" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A118" s="19" t="s">
-        <v>866</v>
+        <v>854</v>
       </c>
       <c r="B118" s="43" t="s">
-        <v>868</v>
+        <v>857</v>
       </c>
       <c r="C118" s="21" t="s">
+        <v>855</v>
+      </c>
+      <c r="D118" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D118" s="23" t="s">
-        <v>867</v>
-      </c>
       <c r="E118" s="26" t="s">
-        <v>868</v>
+        <v>20</v>
       </c>
       <c r="G118" s="29"/>
       <c r="H118" s="23" t="s">
-        <v>867</v>
+        <v>856</v>
       </c>
       <c r="I118" s="26" t="s">
-        <v>869</v>
+        <v>857</v>
       </c>
       <c r="K118" s="29"/>
       <c r="L118" s="31"/>
@@ -7705,64 +7790,48 @@
       <c r="P118" s="29"/>
       <c r="Q118" s="32"/>
       <c r="R118" s="34" t="s">
-        <v>33</v>
+        <v>849</v>
       </c>
     </row>
     <row r="119" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A119" s="19" t="s">
-        <v>870</v>
-      </c>
-      <c r="B119" s="43" t="s">
-        <v>872</v>
-      </c>
-      <c r="C119" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D119" s="23" t="s">
-        <v>871</v>
-      </c>
-      <c r="E119" s="26" t="s">
-        <v>872</v>
-      </c>
+      <c r="A119" s="19"/>
+      <c r="B119" s="39"/>
+      <c r="C119" s="21"/>
+      <c r="D119" s="31"/>
+      <c r="E119" s="33"/>
       <c r="G119" s="29"/>
-      <c r="H119" s="23" t="s">
-        <v>871</v>
-      </c>
-      <c r="I119" s="26" t="s">
-        <v>873</v>
-      </c>
+      <c r="H119" s="31"/>
+      <c r="I119" s="33"/>
       <c r="K119" s="29"/>
       <c r="L119" s="31"/>
       <c r="M119" s="29"/>
       <c r="N119" s="33"/>
       <c r="P119" s="29"/>
       <c r="Q119" s="32"/>
-      <c r="R119" s="34" t="s">
-        <v>33</v>
-      </c>
+      <c r="R119" s="40"/>
     </row>
     <row r="120" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A120" s="19" t="s">
-        <v>874</v>
+      <c r="A120" s="65" t="s">
+        <v>858</v>
       </c>
       <c r="B120" s="43" t="s">
-        <v>876</v>
-      </c>
-      <c r="C120" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D120" s="23" t="s">
-        <v>875</v>
+        <v>860</v>
+      </c>
+      <c r="C120" s="19" t="s">
+        <v>859</v>
+      </c>
+      <c r="D120" s="21" t="s">
+        <v>859</v>
       </c>
       <c r="E120" s="26" t="s">
-        <v>876</v>
-      </c>
-      <c r="G120" s="29"/>
-      <c r="H120" s="23" t="s">
-        <v>875</v>
+        <v>860</v>
+      </c>
+      <c r="G120" s="33"/>
+      <c r="H120" s="21" t="s">
+        <v>859</v>
       </c>
       <c r="I120" s="26" t="s">
-        <v>877</v>
+        <v>861</v>
       </c>
       <c r="K120" s="29"/>
       <c r="L120" s="31"/>
@@ -7770,32 +7839,32 @@
       <c r="N120" s="33"/>
       <c r="P120" s="29"/>
       <c r="Q120" s="32"/>
-      <c r="R120" s="34" t="s">
-        <v>33</v>
+      <c r="R120" s="34" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A121" s="19" t="s">
-        <v>878</v>
+        <v>862</v>
       </c>
       <c r="B121" s="43" t="s">
-        <v>880</v>
+        <v>864</v>
       </c>
       <c r="C121" s="21" t="s">
-        <v>20</v>
+        <v>863</v>
       </c>
       <c r="D121" s="23" t="s">
-        <v>879</v>
+        <v>863</v>
       </c>
       <c r="E121" s="26" t="s">
-        <v>880</v>
+        <v>864</v>
       </c>
       <c r="G121" s="29"/>
       <c r="H121" s="23" t="s">
-        <v>879</v>
+        <v>863</v>
       </c>
       <c r="I121" s="26" t="s">
-        <v>881</v>
+        <v>865</v>
       </c>
       <c r="K121" s="29"/>
       <c r="L121" s="31"/>
@@ -7808,27 +7877,25 @@
       </c>
     </row>
     <row r="122" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A122" s="19" t="s">
-        <v>882</v>
-      </c>
-      <c r="B122" s="43" t="s">
-        <v>884</v>
-      </c>
-      <c r="C122" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D122" s="23" t="s">
-        <v>883</v>
-      </c>
-      <c r="E122" s="26" t="s">
-        <v>884</v>
+      <c r="A122" s="65" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B122" s="68" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C122" s="71"/>
+      <c r="D122" s="66" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E122" s="68" t="s">
+        <v>1143</v>
       </c>
       <c r="G122" s="29"/>
-      <c r="H122" s="23" t="s">
-        <v>883</v>
-      </c>
-      <c r="I122" s="26" t="s">
-        <v>885</v>
+      <c r="H122" s="66" t="s">
+        <v>1142</v>
+      </c>
+      <c r="I122" s="68" t="s">
+        <v>1144</v>
       </c>
       <c r="K122" s="29"/>
       <c r="L122" s="31"/>
@@ -7836,65 +7903,46 @@
       <c r="N122" s="33"/>
       <c r="P122" s="29"/>
       <c r="Q122" s="32"/>
-      <c r="R122" s="34" t="s">
-        <v>33</v>
-      </c>
+      <c r="R122" s="40"/>
     </row>
     <row r="123" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A123" s="19" t="s">
-        <v>886</v>
-      </c>
-      <c r="B123" s="43" t="s">
-        <v>888</v>
-      </c>
-      <c r="C123" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D123" s="23" t="s">
-        <v>887</v>
-      </c>
-      <c r="E123" s="26" t="s">
-        <v>888</v>
-      </c>
+      <c r="A123" s="27"/>
+      <c r="B123" s="39"/>
+      <c r="D123" s="31"/>
+      <c r="E123" s="33"/>
       <c r="G123" s="29"/>
-      <c r="H123" s="23" t="s">
-        <v>887</v>
-      </c>
-      <c r="I123" s="26" t="s">
-        <v>889</v>
-      </c>
+      <c r="H123" s="31"/>
+      <c r="I123" s="33"/>
       <c r="K123" s="29"/>
       <c r="L123" s="31"/>
       <c r="M123" s="29"/>
       <c r="N123" s="33"/>
       <c r="P123" s="29"/>
       <c r="Q123" s="32"/>
-      <c r="R123" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="R123" s="40"/>
     </row>
     <row r="124" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A124" s="19" t="s">
-        <v>890</v>
+        <v>866</v>
       </c>
       <c r="B124" s="43" t="s">
-        <v>892</v>
+        <v>868</v>
       </c>
       <c r="C124" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D124" s="23" t="s">
-        <v>891</v>
+        <v>867</v>
       </c>
       <c r="E124" s="26" t="s">
-        <v>892</v>
+        <v>868</v>
       </c>
       <c r="G124" s="29"/>
       <c r="H124" s="23" t="s">
-        <v>891</v>
+        <v>867</v>
       </c>
       <c r="I124" s="26" t="s">
-        <v>893</v>
+        <v>869</v>
       </c>
       <c r="K124" s="29"/>
       <c r="L124" s="31"/>
@@ -7902,29 +7950,32 @@
       <c r="N124" s="33"/>
       <c r="P124" s="29"/>
       <c r="Q124" s="32"/>
-      <c r="R124" s="34" t="b">
-        <v>1</v>
+      <c r="R124" s="34" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="125" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A125" s="27" t="s">
-        <v>1072</v>
-      </c>
-      <c r="B125" s="69" t="s">
-        <v>1115</v>
-      </c>
-      <c r="D125" s="70" t="s">
-        <v>1073</v>
-      </c>
-      <c r="E125" s="69" t="s">
-        <v>1115</v>
+      <c r="A125" s="19" t="s">
+        <v>870</v>
+      </c>
+      <c r="B125" s="43" t="s">
+        <v>872</v>
+      </c>
+      <c r="C125" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D125" s="23" t="s">
+        <v>871</v>
+      </c>
+      <c r="E125" s="26" t="s">
+        <v>872</v>
       </c>
       <c r="G125" s="29"/>
-      <c r="H125" s="70" t="s">
-        <v>1073</v>
-      </c>
-      <c r="I125" s="69" t="s">
-        <v>1116</v>
+      <c r="H125" s="23" t="s">
+        <v>871</v>
+      </c>
+      <c r="I125" s="26" t="s">
+        <v>873</v>
       </c>
       <c r="K125" s="29"/>
       <c r="L125" s="31"/>
@@ -7932,96 +7983,195 @@
       <c r="N125" s="33"/>
       <c r="P125" s="29"/>
       <c r="Q125" s="32"/>
-      <c r="R125" s="27"/>
+      <c r="R125" s="34" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="126" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A126" s="27"/>
-      <c r="B126" s="39"/>
-      <c r="D126" s="31"/>
-      <c r="E126" s="33"/>
+      <c r="A126" s="19" t="s">
+        <v>874</v>
+      </c>
+      <c r="B126" s="43" t="s">
+        <v>876</v>
+      </c>
+      <c r="C126" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D126" s="23" t="s">
+        <v>875</v>
+      </c>
+      <c r="E126" s="26" t="s">
+        <v>876</v>
+      </c>
       <c r="G126" s="29"/>
-      <c r="H126" s="31"/>
-      <c r="I126" s="33"/>
+      <c r="H126" s="23" t="s">
+        <v>875</v>
+      </c>
+      <c r="I126" s="26" t="s">
+        <v>877</v>
+      </c>
       <c r="K126" s="29"/>
       <c r="L126" s="31"/>
       <c r="M126" s="29"/>
       <c r="N126" s="33"/>
       <c r="P126" s="29"/>
       <c r="Q126" s="32"/>
-      <c r="R126" s="27"/>
+      <c r="R126" s="34" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="127" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A127" s="27"/>
-      <c r="B127" s="39"/>
-      <c r="D127" s="31"/>
-      <c r="E127" s="33"/>
+      <c r="A127" s="19" t="s">
+        <v>878</v>
+      </c>
+      <c r="B127" s="43" t="s">
+        <v>880</v>
+      </c>
+      <c r="C127" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D127" s="23" t="s">
+        <v>879</v>
+      </c>
+      <c r="E127" s="26" t="s">
+        <v>880</v>
+      </c>
       <c r="G127" s="29"/>
-      <c r="H127" s="31"/>
-      <c r="I127" s="33"/>
+      <c r="H127" s="23" t="s">
+        <v>879</v>
+      </c>
+      <c r="I127" s="26" t="s">
+        <v>881</v>
+      </c>
       <c r="K127" s="29"/>
       <c r="L127" s="31"/>
       <c r="M127" s="29"/>
       <c r="N127" s="33"/>
       <c r="P127" s="29"/>
       <c r="Q127" s="32"/>
-      <c r="R127" s="27"/>
+      <c r="R127" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="128" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A128" s="27"/>
-      <c r="B128" s="39"/>
-      <c r="D128" s="31"/>
-      <c r="E128" s="33"/>
+      <c r="A128" s="19" t="s">
+        <v>882</v>
+      </c>
+      <c r="B128" s="43" t="s">
+        <v>884</v>
+      </c>
+      <c r="C128" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D128" s="23" t="s">
+        <v>883</v>
+      </c>
+      <c r="E128" s="26" t="s">
+        <v>884</v>
+      </c>
       <c r="G128" s="29"/>
-      <c r="H128" s="31"/>
-      <c r="I128" s="33"/>
+      <c r="H128" s="23" t="s">
+        <v>883</v>
+      </c>
+      <c r="I128" s="26" t="s">
+        <v>885</v>
+      </c>
       <c r="K128" s="29"/>
       <c r="L128" s="31"/>
       <c r="M128" s="29"/>
       <c r="N128" s="33"/>
       <c r="P128" s="29"/>
       <c r="Q128" s="32"/>
-      <c r="R128" s="27"/>
+      <c r="R128" s="34" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="129" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A129" s="27"/>
-      <c r="B129" s="39"/>
-      <c r="D129" s="31"/>
-      <c r="E129" s="33"/>
+      <c r="A129" s="19" t="s">
+        <v>886</v>
+      </c>
+      <c r="B129" s="43" t="s">
+        <v>888</v>
+      </c>
+      <c r="C129" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D129" s="23" t="s">
+        <v>887</v>
+      </c>
+      <c r="E129" s="26" t="s">
+        <v>888</v>
+      </c>
       <c r="G129" s="29"/>
-      <c r="H129" s="31"/>
-      <c r="I129" s="33"/>
+      <c r="H129" s="23" t="s">
+        <v>887</v>
+      </c>
+      <c r="I129" s="26" t="s">
+        <v>889</v>
+      </c>
       <c r="K129" s="29"/>
       <c r="L129" s="31"/>
       <c r="M129" s="29"/>
       <c r="N129" s="33"/>
       <c r="P129" s="29"/>
       <c r="Q129" s="32"/>
-      <c r="R129" s="27"/>
+      <c r="R129" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="130" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A130" s="27"/>
-      <c r="B130" s="39"/>
-      <c r="D130" s="31"/>
-      <c r="E130" s="33"/>
+      <c r="A130" s="19" t="s">
+        <v>890</v>
+      </c>
+      <c r="B130" s="43" t="s">
+        <v>892</v>
+      </c>
+      <c r="C130" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D130" s="23" t="s">
+        <v>891</v>
+      </c>
+      <c r="E130" s="26" t="s">
+        <v>892</v>
+      </c>
       <c r="G130" s="29"/>
-      <c r="H130" s="31"/>
-      <c r="I130" s="33"/>
+      <c r="H130" s="23" t="s">
+        <v>891</v>
+      </c>
+      <c r="I130" s="26" t="s">
+        <v>893</v>
+      </c>
       <c r="K130" s="29"/>
       <c r="L130" s="31"/>
       <c r="M130" s="29"/>
       <c r="N130" s="33"/>
       <c r="P130" s="29"/>
       <c r="Q130" s="32"/>
-      <c r="R130" s="27"/>
+      <c r="R130" s="34" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="131" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
-      <c r="A131" s="27"/>
-      <c r="B131" s="39"/>
-      <c r="D131" s="31"/>
-      <c r="E131" s="33"/>
+      <c r="A131" s="27" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B131" s="69" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D131" s="70" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E131" s="69" t="s">
+        <v>1115</v>
+      </c>
       <c r="G131" s="29"/>
-      <c r="H131" s="31"/>
-      <c r="I131" s="33"/>
+      <c r="H131" s="70" t="s">
+        <v>1073</v>
+      </c>
+      <c r="I131" s="69" t="s">
+        <v>1116</v>
+      </c>
       <c r="K131" s="29"/>
       <c r="L131" s="31"/>
       <c r="M131" s="29"/>
@@ -22893,6 +23043,102 @@
       <c r="P1060" s="29"/>
       <c r="Q1060" s="32"/>
       <c r="R1060" s="27"/>
+    </row>
+    <row r="1061" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1061" s="27"/>
+      <c r="B1061" s="39"/>
+      <c r="D1061" s="31"/>
+      <c r="E1061" s="33"/>
+      <c r="G1061" s="29"/>
+      <c r="H1061" s="31"/>
+      <c r="I1061" s="33"/>
+      <c r="K1061" s="29"/>
+      <c r="L1061" s="31"/>
+      <c r="M1061" s="29"/>
+      <c r="N1061" s="33"/>
+      <c r="P1061" s="29"/>
+      <c r="Q1061" s="32"/>
+      <c r="R1061" s="27"/>
+    </row>
+    <row r="1062" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1062" s="27"/>
+      <c r="B1062" s="39"/>
+      <c r="D1062" s="31"/>
+      <c r="E1062" s="33"/>
+      <c r="G1062" s="29"/>
+      <c r="H1062" s="31"/>
+      <c r="I1062" s="33"/>
+      <c r="K1062" s="29"/>
+      <c r="L1062" s="31"/>
+      <c r="M1062" s="29"/>
+      <c r="N1062" s="33"/>
+      <c r="P1062" s="29"/>
+      <c r="Q1062" s="32"/>
+      <c r="R1062" s="27"/>
+    </row>
+    <row r="1063" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1063" s="27"/>
+      <c r="B1063" s="39"/>
+      <c r="D1063" s="31"/>
+      <c r="E1063" s="33"/>
+      <c r="G1063" s="29"/>
+      <c r="H1063" s="31"/>
+      <c r="I1063" s="33"/>
+      <c r="K1063" s="29"/>
+      <c r="L1063" s="31"/>
+      <c r="M1063" s="29"/>
+      <c r="N1063" s="33"/>
+      <c r="P1063" s="29"/>
+      <c r="Q1063" s="32"/>
+      <c r="R1063" s="27"/>
+    </row>
+    <row r="1064" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1064" s="27"/>
+      <c r="B1064" s="39"/>
+      <c r="D1064" s="31"/>
+      <c r="E1064" s="33"/>
+      <c r="G1064" s="29"/>
+      <c r="H1064" s="31"/>
+      <c r="I1064" s="33"/>
+      <c r="K1064" s="29"/>
+      <c r="L1064" s="31"/>
+      <c r="M1064" s="29"/>
+      <c r="N1064" s="33"/>
+      <c r="P1064" s="29"/>
+      <c r="Q1064" s="32"/>
+      <c r="R1064" s="27"/>
+    </row>
+    <row r="1065" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1065" s="27"/>
+      <c r="B1065" s="39"/>
+      <c r="D1065" s="31"/>
+      <c r="E1065" s="33"/>
+      <c r="G1065" s="29"/>
+      <c r="H1065" s="31"/>
+      <c r="I1065" s="33"/>
+      <c r="K1065" s="29"/>
+      <c r="L1065" s="31"/>
+      <c r="M1065" s="29"/>
+      <c r="N1065" s="33"/>
+      <c r="P1065" s="29"/>
+      <c r="Q1065" s="32"/>
+      <c r="R1065" s="27"/>
+    </row>
+    <row r="1066" spans="1:18" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="A1066" s="27"/>
+      <c r="B1066" s="39"/>
+      <c r="D1066" s="31"/>
+      <c r="E1066" s="33"/>
+      <c r="G1066" s="29"/>
+      <c r="H1066" s="31"/>
+      <c r="I1066" s="33"/>
+      <c r="K1066" s="29"/>
+      <c r="L1066" s="31"/>
+      <c r="M1066" s="29"/>
+      <c r="N1066" s="33"/>
+      <c r="P1066" s="29"/>
+      <c r="Q1066" s="32"/>
+      <c r="R1066" s="27"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" gridLines="1"/>
@@ -39218,9 +39464,9 @@
   </sheetPr>
   <dimension ref="A1:AB1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D56" sqref="D56"/>
+      <selection pane="topRight" activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -58827,7 +59073,7 @@
   <dimension ref="A1:AB1030"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>